<commit_message>
Daily IST report + updated submissions_daily_matrix.xlsx
</commit_message>
<xml_diff>
--- a/reports/submissions_daily_matrix.xlsx
+++ b/reports/submissions_daily_matrix.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G109"/>
+  <dimension ref="A1:H109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,8 +440,9 @@
     <col width="30" customWidth="1" min="3" max="3"/>
     <col width="12" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
-    <col width="13" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
     <col width="13" customWidth="1" min="7" max="7"/>
+    <col width="13" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -470,12 +471,17 @@
           <t>2026-02-12</t>
         </is>
       </c>
-      <c r="F1" s="2" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>2026-02-13</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
         <is>
           <t>total_files</t>
         </is>
       </c>
-      <c r="G1" s="2" t="inlineStr">
+      <c r="H1" s="2" t="inlineStr">
         <is>
           <t>unique_days</t>
         </is>
@@ -509,6 +515,9 @@
       <c r="G2" t="n">
         <v>0</v>
       </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -538,6 +547,9 @@
       <c r="G3" t="n">
         <v>0</v>
       </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -567,6 +579,9 @@
       <c r="G4" t="n">
         <v>0</v>
       </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -596,6 +611,9 @@
       <c r="G5" t="n">
         <v>0</v>
       </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -625,6 +643,9 @@
       <c r="G6" t="n">
         <v>0</v>
       </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -654,6 +675,9 @@
       <c r="G7" t="n">
         <v>0</v>
       </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -683,6 +707,9 @@
       <c r="G8" t="n">
         <v>0</v>
       </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -712,6 +739,9 @@
       <c r="G9" t="n">
         <v>0</v>
       </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -741,6 +771,9 @@
       <c r="G10" t="n">
         <v>0</v>
       </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -770,6 +803,9 @@
       <c r="G11" t="n">
         <v>0</v>
       </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -799,6 +835,9 @@
       <c r="G12" t="n">
         <v>0</v>
       </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -828,6 +867,9 @@
       <c r="G13" t="n">
         <v>0</v>
       </c>
+      <c r="H13" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -857,6 +899,9 @@
       <c r="G14" t="n">
         <v>0</v>
       </c>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -881,11 +926,14 @@
         <v>1</v>
       </c>
       <c r="F15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15" t="n">
         <v>1</v>
       </c>
+      <c r="H15" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -915,6 +963,9 @@
       <c r="G16" t="n">
         <v>0</v>
       </c>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -944,6 +995,9 @@
       <c r="G17" t="n">
         <v>0</v>
       </c>
+      <c r="H17" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -973,6 +1027,9 @@
       <c r="G18" t="n">
         <v>0</v>
       </c>
+      <c r="H18" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1002,6 +1059,9 @@
       <c r="G19" t="n">
         <v>0</v>
       </c>
+      <c r="H19" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1031,6 +1091,9 @@
       <c r="G20" t="n">
         <v>0</v>
       </c>
+      <c r="H20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1060,6 +1123,9 @@
       <c r="G21" t="n">
         <v>0</v>
       </c>
+      <c r="H21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1089,6 +1155,9 @@
       <c r="G22" t="n">
         <v>0</v>
       </c>
+      <c r="H22" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1118,6 +1187,9 @@
       <c r="G23" t="n">
         <v>0</v>
       </c>
+      <c r="H23" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1147,6 +1219,9 @@
       <c r="G24" t="n">
         <v>0</v>
       </c>
+      <c r="H24" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1176,6 +1251,9 @@
       <c r="G25" t="n">
         <v>0</v>
       </c>
+      <c r="H25" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1205,6 +1283,9 @@
       <c r="G26" t="n">
         <v>0</v>
       </c>
+      <c r="H26" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1234,6 +1315,9 @@
       <c r="G27" t="n">
         <v>0</v>
       </c>
+      <c r="H27" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1263,6 +1347,9 @@
       <c r="G28" t="n">
         <v>0</v>
       </c>
+      <c r="H28" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1292,6 +1379,9 @@
       <c r="G29" t="n">
         <v>0</v>
       </c>
+      <c r="H29" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1321,6 +1411,9 @@
       <c r="G30" t="n">
         <v>0</v>
       </c>
+      <c r="H30" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1350,6 +1443,9 @@
       <c r="G31" t="n">
         <v>0</v>
       </c>
+      <c r="H31" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1379,6 +1475,9 @@
       <c r="G32" t="n">
         <v>0</v>
       </c>
+      <c r="H32" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1408,6 +1507,9 @@
       <c r="G33" t="n">
         <v>0</v>
       </c>
+      <c r="H33" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1437,6 +1539,9 @@
       <c r="G34" t="n">
         <v>0</v>
       </c>
+      <c r="H34" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1466,6 +1571,9 @@
       <c r="G35" t="n">
         <v>0</v>
       </c>
+      <c r="H35" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1495,6 +1603,9 @@
       <c r="G36" t="n">
         <v>0</v>
       </c>
+      <c r="H36" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1524,6 +1635,9 @@
       <c r="G37" t="n">
         <v>0</v>
       </c>
+      <c r="H37" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1553,6 +1667,9 @@
       <c r="G38" t="n">
         <v>0</v>
       </c>
+      <c r="H38" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1582,6 +1699,9 @@
       <c r="G39" t="n">
         <v>0</v>
       </c>
+      <c r="H39" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1611,6 +1731,9 @@
       <c r="G40" t="n">
         <v>0</v>
       </c>
+      <c r="H40" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1640,6 +1763,9 @@
       <c r="G41" t="n">
         <v>0</v>
       </c>
+      <c r="H41" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1669,6 +1795,9 @@
       <c r="G42" t="n">
         <v>0</v>
       </c>
+      <c r="H42" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1698,6 +1827,9 @@
       <c r="G43" t="n">
         <v>0</v>
       </c>
+      <c r="H43" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1727,6 +1859,9 @@
       <c r="G44" t="n">
         <v>0</v>
       </c>
+      <c r="H44" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1756,6 +1891,9 @@
       <c r="G45" t="n">
         <v>0</v>
       </c>
+      <c r="H45" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1785,6 +1923,9 @@
       <c r="G46" t="n">
         <v>0</v>
       </c>
+      <c r="H46" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1814,6 +1955,9 @@
       <c r="G47" t="n">
         <v>0</v>
       </c>
+      <c r="H47" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1843,6 +1987,9 @@
       <c r="G48" t="n">
         <v>0</v>
       </c>
+      <c r="H48" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1872,6 +2019,9 @@
       <c r="G49" t="n">
         <v>0</v>
       </c>
+      <c r="H49" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1901,6 +2051,9 @@
       <c r="G50" t="n">
         <v>0</v>
       </c>
+      <c r="H50" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1930,6 +2083,9 @@
       <c r="G51" t="n">
         <v>0</v>
       </c>
+      <c r="H51" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1959,6 +2115,9 @@
       <c r="G52" t="n">
         <v>0</v>
       </c>
+      <c r="H52" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1988,6 +2147,9 @@
       <c r="G53" t="n">
         <v>0</v>
       </c>
+      <c r="H53" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -2017,6 +2179,9 @@
       <c r="G54" t="n">
         <v>0</v>
       </c>
+      <c r="H54" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -2046,6 +2211,9 @@
       <c r="G55" t="n">
         <v>0</v>
       </c>
+      <c r="H55" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -2075,6 +2243,9 @@
       <c r="G56" t="n">
         <v>0</v>
       </c>
+      <c r="H56" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -2104,6 +2275,9 @@
       <c r="G57" t="n">
         <v>0</v>
       </c>
+      <c r="H57" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -2133,6 +2307,9 @@
       <c r="G58" t="n">
         <v>0</v>
       </c>
+      <c r="H58" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -2162,6 +2339,9 @@
       <c r="G59" t="n">
         <v>0</v>
       </c>
+      <c r="H59" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -2191,6 +2371,9 @@
       <c r="G60" t="n">
         <v>0</v>
       </c>
+      <c r="H60" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -2220,6 +2403,9 @@
       <c r="G61" t="n">
         <v>0</v>
       </c>
+      <c r="H61" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -2249,6 +2435,9 @@
       <c r="G62" t="n">
         <v>0</v>
       </c>
+      <c r="H62" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -2278,6 +2467,9 @@
       <c r="G63" t="n">
         <v>0</v>
       </c>
+      <c r="H63" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2307,6 +2499,9 @@
       <c r="G64" t="n">
         <v>0</v>
       </c>
+      <c r="H64" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -2336,6 +2531,9 @@
       <c r="G65" t="n">
         <v>0</v>
       </c>
+      <c r="H65" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -2365,6 +2563,9 @@
       <c r="G66" t="n">
         <v>0</v>
       </c>
+      <c r="H66" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -2394,6 +2595,9 @@
       <c r="G67" t="n">
         <v>0</v>
       </c>
+      <c r="H67" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -2423,6 +2627,9 @@
       <c r="G68" t="n">
         <v>0</v>
       </c>
+      <c r="H68" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -2452,6 +2659,9 @@
       <c r="G69" t="n">
         <v>0</v>
       </c>
+      <c r="H69" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -2481,6 +2691,9 @@
       <c r="G70" t="n">
         <v>0</v>
       </c>
+      <c r="H70" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -2510,6 +2723,9 @@
       <c r="G71" t="n">
         <v>0</v>
       </c>
+      <c r="H71" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -2539,6 +2755,9 @@
       <c r="G72" t="n">
         <v>0</v>
       </c>
+      <c r="H72" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -2568,6 +2787,9 @@
       <c r="G73" t="n">
         <v>0</v>
       </c>
+      <c r="H73" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -2597,6 +2819,9 @@
       <c r="G74" t="n">
         <v>0</v>
       </c>
+      <c r="H74" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -2626,6 +2851,9 @@
       <c r="G75" t="n">
         <v>0</v>
       </c>
+      <c r="H75" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -2655,6 +2883,9 @@
       <c r="G76" t="n">
         <v>0</v>
       </c>
+      <c r="H76" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -2684,6 +2915,9 @@
       <c r="G77" t="n">
         <v>0</v>
       </c>
+      <c r="H77" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -2713,6 +2947,9 @@
       <c r="G78" t="n">
         <v>0</v>
       </c>
+      <c r="H78" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -2742,6 +2979,9 @@
       <c r="G79" t="n">
         <v>0</v>
       </c>
+      <c r="H79" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -2771,6 +3011,9 @@
       <c r="G80" t="n">
         <v>0</v>
       </c>
+      <c r="H80" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -2800,6 +3043,9 @@
       <c r="G81" t="n">
         <v>0</v>
       </c>
+      <c r="H81" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -2829,6 +3075,9 @@
       <c r="G82" t="n">
         <v>0</v>
       </c>
+      <c r="H82" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -2858,6 +3107,9 @@
       <c r="G83" t="n">
         <v>0</v>
       </c>
+      <c r="H83" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -2887,6 +3139,9 @@
       <c r="G84" t="n">
         <v>0</v>
       </c>
+      <c r="H84" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -2916,6 +3171,9 @@
       <c r="G85" t="n">
         <v>0</v>
       </c>
+      <c r="H85" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -2945,6 +3203,9 @@
       <c r="G86" t="n">
         <v>0</v>
       </c>
+      <c r="H86" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -2974,6 +3235,9 @@
       <c r="G87" t="n">
         <v>0</v>
       </c>
+      <c r="H87" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -3003,6 +3267,9 @@
       <c r="G88" t="n">
         <v>0</v>
       </c>
+      <c r="H88" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -3032,6 +3299,9 @@
       <c r="G89" t="n">
         <v>0</v>
       </c>
+      <c r="H89" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -3061,6 +3331,9 @@
       <c r="G90" t="n">
         <v>0</v>
       </c>
+      <c r="H90" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -3090,6 +3363,9 @@
       <c r="G91" t="n">
         <v>0</v>
       </c>
+      <c r="H91" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -3119,6 +3395,9 @@
       <c r="G92" t="n">
         <v>0</v>
       </c>
+      <c r="H92" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -3148,6 +3427,9 @@
       <c r="G93" t="n">
         <v>0</v>
       </c>
+      <c r="H93" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -3177,6 +3459,9 @@
       <c r="G94" t="n">
         <v>0</v>
       </c>
+      <c r="H94" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -3206,6 +3491,9 @@
       <c r="G95" t="n">
         <v>0</v>
       </c>
+      <c r="H95" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -3235,6 +3523,9 @@
       <c r="G96" t="n">
         <v>0</v>
       </c>
+      <c r="H96" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -3264,6 +3555,9 @@
       <c r="G97" t="n">
         <v>0</v>
       </c>
+      <c r="H97" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -3293,6 +3587,9 @@
       <c r="G98" t="n">
         <v>0</v>
       </c>
+      <c r="H98" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -3322,6 +3619,9 @@
       <c r="G99" t="n">
         <v>0</v>
       </c>
+      <c r="H99" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -3351,6 +3651,9 @@
       <c r="G100" t="n">
         <v>0</v>
       </c>
+      <c r="H100" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -3380,6 +3683,9 @@
       <c r="G101" t="n">
         <v>0</v>
       </c>
+      <c r="H101" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -3409,6 +3715,9 @@
       <c r="G102" t="n">
         <v>0</v>
       </c>
+      <c r="H102" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -3438,6 +3747,9 @@
       <c r="G103" t="n">
         <v>0</v>
       </c>
+      <c r="H103" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -3467,6 +3779,9 @@
       <c r="G104" t="n">
         <v>0</v>
       </c>
+      <c r="H104" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -3496,6 +3811,9 @@
       <c r="G105" t="n">
         <v>0</v>
       </c>
+      <c r="H105" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -3525,6 +3843,9 @@
       <c r="G106" t="n">
         <v>0</v>
       </c>
+      <c r="H106" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -3554,6 +3875,9 @@
       <c r="G107" t="n">
         <v>0</v>
       </c>
+      <c r="H107" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -3583,6 +3907,9 @@
       <c r="G108" t="n">
         <v>0</v>
       </c>
+      <c r="H108" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -3610,6 +3937,9 @@
         <v>0</v>
       </c>
       <c r="G109" t="n">
+        <v>0</v>
+      </c>
+      <c r="H109" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Daily IST report: add CSV/MD/XLSX
</commit_message>
<xml_diff>
--- a/reports/submissions_daily_matrix.xlsx
+++ b/reports/submissions_daily_matrix.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H109"/>
+  <dimension ref="A1:I109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,8 +441,9 @@
     <col width="12" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
     <col width="12" customWidth="1" min="6" max="6"/>
-    <col width="13" customWidth="1" min="7" max="7"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
     <col width="13" customWidth="1" min="8" max="8"/>
+    <col width="13" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -476,12 +477,17 @@
           <t>2026-02-13</t>
         </is>
       </c>
-      <c r="G1" s="2" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>2026-02-18</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="inlineStr">
         <is>
           <t>total_files</t>
         </is>
       </c>
-      <c r="H1" s="2" t="inlineStr">
+      <c r="I1" s="2" t="inlineStr">
         <is>
           <t>unique_days</t>
         </is>
@@ -513,10 +519,13 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -545,10 +554,13 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I3" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -582,6 +594,9 @@
       <c r="H4" t="n">
         <v>0</v>
       </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -609,10 +624,13 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -646,6 +664,9 @@
       <c r="H6" t="n">
         <v>0</v>
       </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -673,10 +694,13 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I7" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -705,10 +729,13 @@
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I8" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -737,10 +764,13 @@
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I9" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -769,10 +799,13 @@
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I10" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -806,6 +839,9 @@
       <c r="H11" t="n">
         <v>0</v>
       </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -833,10 +869,13 @@
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I12" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -865,10 +904,13 @@
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I13" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="14">
@@ -897,10 +939,13 @@
         <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I14" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="15">
@@ -929,9 +974,12 @@
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" t="n">
+        <v>1</v>
+      </c>
+      <c r="I15" t="n">
         <v>1</v>
       </c>
     </row>
@@ -966,6 +1014,9 @@
       <c r="H16" t="n">
         <v>0</v>
       </c>
+      <c r="I16" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -993,10 +1044,13 @@
         <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I17" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -1025,10 +1079,13 @@
         <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I18" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="19">
@@ -1057,10 +1114,13 @@
         <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I19" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="20">
@@ -1089,10 +1149,13 @@
         <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I20" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="21">
@@ -1126,6 +1189,9 @@
       <c r="H21" t="n">
         <v>0</v>
       </c>
+      <c r="I21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1158,6 +1224,9 @@
       <c r="H22" t="n">
         <v>0</v>
       </c>
+      <c r="I22" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1190,6 +1259,9 @@
       <c r="H23" t="n">
         <v>0</v>
       </c>
+      <c r="I23" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1217,10 +1289,13 @@
         <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I24" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="25">
@@ -1249,10 +1324,13 @@
         <v>0</v>
       </c>
       <c r="G25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I25" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="26">
@@ -1286,6 +1364,9 @@
       <c r="H26" t="n">
         <v>0</v>
       </c>
+      <c r="I26" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1313,10 +1394,13 @@
         <v>0</v>
       </c>
       <c r="G27" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H27" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="I27" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="28">
@@ -1350,6 +1434,9 @@
       <c r="H28" t="n">
         <v>0</v>
       </c>
+      <c r="I28" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1382,6 +1469,9 @@
       <c r="H29" t="n">
         <v>0</v>
       </c>
+      <c r="I29" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1414,6 +1504,9 @@
       <c r="H30" t="n">
         <v>0</v>
       </c>
+      <c r="I30" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1441,10 +1534,13 @@
         <v>0</v>
       </c>
       <c r="G31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H31" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I31" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="32">
@@ -1473,10 +1569,13 @@
         <v>0</v>
       </c>
       <c r="G32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H32" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I32" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="33">
@@ -1505,10 +1604,13 @@
         <v>0</v>
       </c>
       <c r="G33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H33" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I33" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="34">
@@ -1537,10 +1639,13 @@
         <v>0</v>
       </c>
       <c r="G34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H34" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I34" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="35">
@@ -1569,10 +1674,13 @@
         <v>0</v>
       </c>
       <c r="G35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H35" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I35" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="36">
@@ -1606,6 +1714,9 @@
       <c r="H36" t="n">
         <v>0</v>
       </c>
+      <c r="I36" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1633,10 +1744,13 @@
         <v>0</v>
       </c>
       <c r="G37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H37" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I37" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="38">
@@ -1670,6 +1784,9 @@
       <c r="H38" t="n">
         <v>0</v>
       </c>
+      <c r="I38" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1702,6 +1819,9 @@
       <c r="H39" t="n">
         <v>0</v>
       </c>
+      <c r="I39" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1729,10 +1849,13 @@
         <v>0</v>
       </c>
       <c r="G40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H40" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I40" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="41">
@@ -1761,10 +1884,13 @@
         <v>0</v>
       </c>
       <c r="G41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H41" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I41" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="42">
@@ -1793,10 +1919,13 @@
         <v>0</v>
       </c>
       <c r="G42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H42" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I42" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="43">
@@ -1825,10 +1954,13 @@
         <v>0</v>
       </c>
       <c r="G43" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="H43" t="n">
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="I43" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="44">
@@ -1862,6 +1994,9 @@
       <c r="H44" t="n">
         <v>0</v>
       </c>
+      <c r="I44" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1889,10 +2024,13 @@
         <v>0</v>
       </c>
       <c r="G45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H45" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I45" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="46">
@@ -1921,10 +2059,13 @@
         <v>0</v>
       </c>
       <c r="G46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H46" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I46" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="47">
@@ -1953,10 +2094,13 @@
         <v>0</v>
       </c>
       <c r="G47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H47" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I47" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="48">
@@ -1990,6 +2134,9 @@
       <c r="H48" t="n">
         <v>0</v>
       </c>
+      <c r="I48" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2017,10 +2164,13 @@
         <v>0</v>
       </c>
       <c r="G49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H49" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I49" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="50">
@@ -2054,6 +2204,9 @@
       <c r="H50" t="n">
         <v>0</v>
       </c>
+      <c r="I50" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -2086,6 +2239,9 @@
       <c r="H51" t="n">
         <v>0</v>
       </c>
+      <c r="I51" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -2113,10 +2269,13 @@
         <v>0</v>
       </c>
       <c r="G52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H52" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I52" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="53">
@@ -2150,6 +2309,9 @@
       <c r="H53" t="n">
         <v>0</v>
       </c>
+      <c r="I53" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -2182,6 +2344,9 @@
       <c r="H54" t="n">
         <v>0</v>
       </c>
+      <c r="I54" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -2209,10 +2374,13 @@
         <v>0</v>
       </c>
       <c r="G55" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H55" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I55" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="56">
@@ -2246,6 +2414,9 @@
       <c r="H56" t="n">
         <v>0</v>
       </c>
+      <c r="I56" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -2278,6 +2449,9 @@
       <c r="H57" t="n">
         <v>0</v>
       </c>
+      <c r="I57" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -2305,10 +2479,13 @@
         <v>0</v>
       </c>
       <c r="G58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H58" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I58" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="59">
@@ -2342,6 +2519,9 @@
       <c r="H59" t="n">
         <v>0</v>
       </c>
+      <c r="I59" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -2369,10 +2549,13 @@
         <v>0</v>
       </c>
       <c r="G60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H60" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I60" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="61">
@@ -2401,10 +2584,13 @@
         <v>0</v>
       </c>
       <c r="G61" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H61" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I61" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="62">
@@ -2438,6 +2624,9 @@
       <c r="H62" t="n">
         <v>0</v>
       </c>
+      <c r="I62" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -2470,6 +2659,9 @@
       <c r="H63" t="n">
         <v>0</v>
       </c>
+      <c r="I63" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2497,10 +2689,13 @@
         <v>0</v>
       </c>
       <c r="G64" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H64" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I64" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="65">
@@ -2534,6 +2729,9 @@
       <c r="H65" t="n">
         <v>0</v>
       </c>
+      <c r="I65" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -2566,6 +2764,9 @@
       <c r="H66" t="n">
         <v>0</v>
       </c>
+      <c r="I66" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -2598,6 +2799,9 @@
       <c r="H67" t="n">
         <v>0</v>
       </c>
+      <c r="I67" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -2630,6 +2834,9 @@
       <c r="H68" t="n">
         <v>0</v>
       </c>
+      <c r="I68" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -2662,6 +2869,9 @@
       <c r="H69" t="n">
         <v>0</v>
       </c>
+      <c r="I69" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -2689,10 +2899,13 @@
         <v>0</v>
       </c>
       <c r="G70" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H70" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I70" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="71">
@@ -2726,6 +2939,9 @@
       <c r="H71" t="n">
         <v>0</v>
       </c>
+      <c r="I71" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -2758,6 +2974,9 @@
       <c r="H72" t="n">
         <v>0</v>
       </c>
+      <c r="I72" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -2790,6 +3009,9 @@
       <c r="H73" t="n">
         <v>0</v>
       </c>
+      <c r="I73" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -2817,10 +3039,13 @@
         <v>0</v>
       </c>
       <c r="G74" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="H74" t="n">
-        <v>0</v>
+        <v>13</v>
+      </c>
+      <c r="I74" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="75">
@@ -2854,6 +3079,9 @@
       <c r="H75" t="n">
         <v>0</v>
       </c>
+      <c r="I75" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -2881,10 +3109,13 @@
         <v>0</v>
       </c>
       <c r="G76" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H76" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I76" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="77">
@@ -2918,6 +3149,9 @@
       <c r="H77" t="n">
         <v>0</v>
       </c>
+      <c r="I77" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -2950,6 +3184,9 @@
       <c r="H78" t="n">
         <v>0</v>
       </c>
+      <c r="I78" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -2982,6 +3219,9 @@
       <c r="H79" t="n">
         <v>0</v>
       </c>
+      <c r="I79" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -3014,6 +3254,9 @@
       <c r="H80" t="n">
         <v>0</v>
       </c>
+      <c r="I80" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -3046,6 +3289,9 @@
       <c r="H81" t="n">
         <v>0</v>
       </c>
+      <c r="I81" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -3073,10 +3319,13 @@
         <v>0</v>
       </c>
       <c r="G82" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H82" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I82" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="83">
@@ -3110,6 +3359,9 @@
       <c r="H83" t="n">
         <v>0</v>
       </c>
+      <c r="I83" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -3137,10 +3389,13 @@
         <v>0</v>
       </c>
       <c r="G84" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H84" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I84" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="85">
@@ -3174,6 +3429,9 @@
       <c r="H85" t="n">
         <v>0</v>
       </c>
+      <c r="I85" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -3201,10 +3459,13 @@
         <v>0</v>
       </c>
       <c r="G86" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H86" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I86" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="87">
@@ -3238,6 +3499,9 @@
       <c r="H87" t="n">
         <v>0</v>
       </c>
+      <c r="I87" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -3270,6 +3534,9 @@
       <c r="H88" t="n">
         <v>0</v>
       </c>
+      <c r="I88" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -3302,6 +3569,9 @@
       <c r="H89" t="n">
         <v>0</v>
       </c>
+      <c r="I89" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -3334,6 +3604,9 @@
       <c r="H90" t="n">
         <v>0</v>
       </c>
+      <c r="I90" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -3366,6 +3639,9 @@
       <c r="H91" t="n">
         <v>0</v>
       </c>
+      <c r="I91" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -3398,6 +3674,9 @@
       <c r="H92" t="n">
         <v>0</v>
       </c>
+      <c r="I92" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -3430,6 +3709,9 @@
       <c r="H93" t="n">
         <v>0</v>
       </c>
+      <c r="I93" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -3462,6 +3744,9 @@
       <c r="H94" t="n">
         <v>0</v>
       </c>
+      <c r="I94" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -3489,10 +3774,13 @@
         <v>0</v>
       </c>
       <c r="G95" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="H95" t="n">
-        <v>0</v>
+        <v>30</v>
+      </c>
+      <c r="I95" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="96">
@@ -3526,6 +3814,9 @@
       <c r="H96" t="n">
         <v>0</v>
       </c>
+      <c r="I96" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -3558,6 +3849,9 @@
       <c r="H97" t="n">
         <v>0</v>
       </c>
+      <c r="I97" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -3590,6 +3884,9 @@
       <c r="H98" t="n">
         <v>0</v>
       </c>
+      <c r="I98" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -3622,6 +3919,9 @@
       <c r="H99" t="n">
         <v>0</v>
       </c>
+      <c r="I99" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -3649,10 +3949,13 @@
         <v>0</v>
       </c>
       <c r="G100" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H100" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I100" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="101">
@@ -3681,10 +3984,13 @@
         <v>0</v>
       </c>
       <c r="G101" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H101" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I101" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="102">
@@ -3718,6 +4024,9 @@
       <c r="H102" t="n">
         <v>0</v>
       </c>
+      <c r="I102" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -3745,10 +4054,13 @@
         <v>0</v>
       </c>
       <c r="G103" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H103" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I103" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="104">
@@ -3777,10 +4089,13 @@
         <v>0</v>
       </c>
       <c r="G104" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H104" t="n">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="I104" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="105">
@@ -3809,10 +4124,13 @@
         <v>0</v>
       </c>
       <c r="G105" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H105" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I105" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="106">
@@ -3841,10 +4159,13 @@
         <v>0</v>
       </c>
       <c r="G106" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H106" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I106" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="107">
@@ -3878,6 +4199,9 @@
       <c r="H107" t="n">
         <v>0</v>
       </c>
+      <c r="I107" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -3905,10 +4229,13 @@
         <v>0</v>
       </c>
       <c r="G108" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H108" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I108" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="109">
@@ -3940,6 +4267,9 @@
         <v>0</v>
       </c>
       <c r="H109" t="n">
+        <v>0</v>
+      </c>
+      <c r="I109" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Daily IST report: add CSV/MD/XLSX (#270)
Co-authored-by: codethesept <198977775+codethesept@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/reports/submissions_daily_matrix.xlsx
+++ b/reports/submissions_daily_matrix.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H109"/>
+  <dimension ref="A1:I109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,8 +441,9 @@
     <col width="12" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
     <col width="12" customWidth="1" min="6" max="6"/>
-    <col width="13" customWidth="1" min="7" max="7"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
     <col width="13" customWidth="1" min="8" max="8"/>
+    <col width="13" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -476,12 +477,17 @@
           <t>2026-02-13</t>
         </is>
       </c>
-      <c r="G1" s="2" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>2026-02-18</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="inlineStr">
         <is>
           <t>total_files</t>
         </is>
       </c>
-      <c r="H1" s="2" t="inlineStr">
+      <c r="I1" s="2" t="inlineStr">
         <is>
           <t>unique_days</t>
         </is>
@@ -513,10 +519,13 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -545,10 +554,13 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I3" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -582,6 +594,9 @@
       <c r="H4" t="n">
         <v>0</v>
       </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -609,10 +624,13 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -646,6 +664,9 @@
       <c r="H6" t="n">
         <v>0</v>
       </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -673,10 +694,13 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I7" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -705,10 +729,13 @@
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I8" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -737,10 +764,13 @@
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I9" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -769,10 +799,13 @@
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I10" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -806,6 +839,9 @@
       <c r="H11" t="n">
         <v>0</v>
       </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -833,10 +869,13 @@
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I12" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -865,10 +904,13 @@
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I13" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="14">
@@ -897,10 +939,13 @@
         <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I14" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="15">
@@ -929,9 +974,12 @@
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" t="n">
+        <v>1</v>
+      </c>
+      <c r="I15" t="n">
         <v>1</v>
       </c>
     </row>
@@ -966,6 +1014,9 @@
       <c r="H16" t="n">
         <v>0</v>
       </c>
+      <c r="I16" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -993,10 +1044,13 @@
         <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I17" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -1025,10 +1079,13 @@
         <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I18" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="19">
@@ -1057,10 +1114,13 @@
         <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I19" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="20">
@@ -1089,10 +1149,13 @@
         <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I20" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="21">
@@ -1126,6 +1189,9 @@
       <c r="H21" t="n">
         <v>0</v>
       </c>
+      <c r="I21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1158,6 +1224,9 @@
       <c r="H22" t="n">
         <v>0</v>
       </c>
+      <c r="I22" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1190,6 +1259,9 @@
       <c r="H23" t="n">
         <v>0</v>
       </c>
+      <c r="I23" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1217,10 +1289,13 @@
         <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I24" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="25">
@@ -1249,10 +1324,13 @@
         <v>0</v>
       </c>
       <c r="G25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I25" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="26">
@@ -1286,6 +1364,9 @@
       <c r="H26" t="n">
         <v>0</v>
       </c>
+      <c r="I26" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1313,10 +1394,13 @@
         <v>0</v>
       </c>
       <c r="G27" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H27" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="I27" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="28">
@@ -1350,6 +1434,9 @@
       <c r="H28" t="n">
         <v>0</v>
       </c>
+      <c r="I28" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1382,6 +1469,9 @@
       <c r="H29" t="n">
         <v>0</v>
       </c>
+      <c r="I29" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1414,6 +1504,9 @@
       <c r="H30" t="n">
         <v>0</v>
       </c>
+      <c r="I30" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1441,10 +1534,13 @@
         <v>0</v>
       </c>
       <c r="G31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H31" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I31" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="32">
@@ -1473,10 +1569,13 @@
         <v>0</v>
       </c>
       <c r="G32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H32" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I32" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="33">
@@ -1505,10 +1604,13 @@
         <v>0</v>
       </c>
       <c r="G33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H33" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I33" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="34">
@@ -1537,10 +1639,13 @@
         <v>0</v>
       </c>
       <c r="G34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H34" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I34" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="35">
@@ -1569,10 +1674,13 @@
         <v>0</v>
       </c>
       <c r="G35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H35" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I35" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="36">
@@ -1606,6 +1714,9 @@
       <c r="H36" t="n">
         <v>0</v>
       </c>
+      <c r="I36" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1633,10 +1744,13 @@
         <v>0</v>
       </c>
       <c r="G37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H37" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I37" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="38">
@@ -1670,6 +1784,9 @@
       <c r="H38" t="n">
         <v>0</v>
       </c>
+      <c r="I38" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1702,6 +1819,9 @@
       <c r="H39" t="n">
         <v>0</v>
       </c>
+      <c r="I39" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1729,10 +1849,13 @@
         <v>0</v>
       </c>
       <c r="G40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H40" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I40" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="41">
@@ -1761,10 +1884,13 @@
         <v>0</v>
       </c>
       <c r="G41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H41" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I41" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="42">
@@ -1793,10 +1919,13 @@
         <v>0</v>
       </c>
       <c r="G42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H42" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I42" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="43">
@@ -1825,10 +1954,13 @@
         <v>0</v>
       </c>
       <c r="G43" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="H43" t="n">
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="I43" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="44">
@@ -1862,6 +1994,9 @@
       <c r="H44" t="n">
         <v>0</v>
       </c>
+      <c r="I44" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1889,10 +2024,13 @@
         <v>0</v>
       </c>
       <c r="G45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H45" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I45" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="46">
@@ -1921,10 +2059,13 @@
         <v>0</v>
       </c>
       <c r="G46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H46" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I46" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="47">
@@ -1953,10 +2094,13 @@
         <v>0</v>
       </c>
       <c r="G47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H47" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I47" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="48">
@@ -1990,6 +2134,9 @@
       <c r="H48" t="n">
         <v>0</v>
       </c>
+      <c r="I48" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2017,10 +2164,13 @@
         <v>0</v>
       </c>
       <c r="G49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H49" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I49" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="50">
@@ -2054,6 +2204,9 @@
       <c r="H50" t="n">
         <v>0</v>
       </c>
+      <c r="I50" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -2086,6 +2239,9 @@
       <c r="H51" t="n">
         <v>0</v>
       </c>
+      <c r="I51" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -2113,10 +2269,13 @@
         <v>0</v>
       </c>
       <c r="G52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H52" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I52" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="53">
@@ -2150,6 +2309,9 @@
       <c r="H53" t="n">
         <v>0</v>
       </c>
+      <c r="I53" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -2182,6 +2344,9 @@
       <c r="H54" t="n">
         <v>0</v>
       </c>
+      <c r="I54" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -2209,10 +2374,13 @@
         <v>0</v>
       </c>
       <c r="G55" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H55" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I55" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="56">
@@ -2246,6 +2414,9 @@
       <c r="H56" t="n">
         <v>0</v>
       </c>
+      <c r="I56" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -2278,6 +2449,9 @@
       <c r="H57" t="n">
         <v>0</v>
       </c>
+      <c r="I57" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -2305,10 +2479,13 @@
         <v>0</v>
       </c>
       <c r="G58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H58" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I58" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="59">
@@ -2342,6 +2519,9 @@
       <c r="H59" t="n">
         <v>0</v>
       </c>
+      <c r="I59" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -2369,10 +2549,13 @@
         <v>0</v>
       </c>
       <c r="G60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H60" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I60" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="61">
@@ -2401,10 +2584,13 @@
         <v>0</v>
       </c>
       <c r="G61" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H61" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I61" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="62">
@@ -2438,6 +2624,9 @@
       <c r="H62" t="n">
         <v>0</v>
       </c>
+      <c r="I62" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -2470,6 +2659,9 @@
       <c r="H63" t="n">
         <v>0</v>
       </c>
+      <c r="I63" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2497,10 +2689,13 @@
         <v>0</v>
       </c>
       <c r="G64" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H64" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I64" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="65">
@@ -2534,6 +2729,9 @@
       <c r="H65" t="n">
         <v>0</v>
       </c>
+      <c r="I65" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -2566,6 +2764,9 @@
       <c r="H66" t="n">
         <v>0</v>
       </c>
+      <c r="I66" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -2598,6 +2799,9 @@
       <c r="H67" t="n">
         <v>0</v>
       </c>
+      <c r="I67" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -2630,6 +2834,9 @@
       <c r="H68" t="n">
         <v>0</v>
       </c>
+      <c r="I68" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -2662,6 +2869,9 @@
       <c r="H69" t="n">
         <v>0</v>
       </c>
+      <c r="I69" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -2689,10 +2899,13 @@
         <v>0</v>
       </c>
       <c r="G70" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H70" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I70" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="71">
@@ -2726,6 +2939,9 @@
       <c r="H71" t="n">
         <v>0</v>
       </c>
+      <c r="I71" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -2758,6 +2974,9 @@
       <c r="H72" t="n">
         <v>0</v>
       </c>
+      <c r="I72" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -2790,6 +3009,9 @@
       <c r="H73" t="n">
         <v>0</v>
       </c>
+      <c r="I73" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -2817,10 +3039,13 @@
         <v>0</v>
       </c>
       <c r="G74" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="H74" t="n">
-        <v>0</v>
+        <v>13</v>
+      </c>
+      <c r="I74" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="75">
@@ -2854,6 +3079,9 @@
       <c r="H75" t="n">
         <v>0</v>
       </c>
+      <c r="I75" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -2881,10 +3109,13 @@
         <v>0</v>
       </c>
       <c r="G76" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H76" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I76" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="77">
@@ -2918,6 +3149,9 @@
       <c r="H77" t="n">
         <v>0</v>
       </c>
+      <c r="I77" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -2950,6 +3184,9 @@
       <c r="H78" t="n">
         <v>0</v>
       </c>
+      <c r="I78" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -2982,6 +3219,9 @@
       <c r="H79" t="n">
         <v>0</v>
       </c>
+      <c r="I79" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -3014,6 +3254,9 @@
       <c r="H80" t="n">
         <v>0</v>
       </c>
+      <c r="I80" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -3046,6 +3289,9 @@
       <c r="H81" t="n">
         <v>0</v>
       </c>
+      <c r="I81" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -3073,10 +3319,13 @@
         <v>0</v>
       </c>
       <c r="G82" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H82" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I82" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="83">
@@ -3110,6 +3359,9 @@
       <c r="H83" t="n">
         <v>0</v>
       </c>
+      <c r="I83" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -3137,10 +3389,13 @@
         <v>0</v>
       </c>
       <c r="G84" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H84" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I84" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="85">
@@ -3174,6 +3429,9 @@
       <c r="H85" t="n">
         <v>0</v>
       </c>
+      <c r="I85" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -3201,10 +3459,13 @@
         <v>0</v>
       </c>
       <c r="G86" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H86" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I86" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="87">
@@ -3238,6 +3499,9 @@
       <c r="H87" t="n">
         <v>0</v>
       </c>
+      <c r="I87" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -3270,6 +3534,9 @@
       <c r="H88" t="n">
         <v>0</v>
       </c>
+      <c r="I88" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -3302,6 +3569,9 @@
       <c r="H89" t="n">
         <v>0</v>
       </c>
+      <c r="I89" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -3334,6 +3604,9 @@
       <c r="H90" t="n">
         <v>0</v>
       </c>
+      <c r="I90" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -3366,6 +3639,9 @@
       <c r="H91" t="n">
         <v>0</v>
       </c>
+      <c r="I91" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -3398,6 +3674,9 @@
       <c r="H92" t="n">
         <v>0</v>
       </c>
+      <c r="I92" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -3430,6 +3709,9 @@
       <c r="H93" t="n">
         <v>0</v>
       </c>
+      <c r="I93" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -3462,6 +3744,9 @@
       <c r="H94" t="n">
         <v>0</v>
       </c>
+      <c r="I94" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -3489,10 +3774,13 @@
         <v>0</v>
       </c>
       <c r="G95" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="H95" t="n">
-        <v>0</v>
+        <v>30</v>
+      </c>
+      <c r="I95" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="96">
@@ -3526,6 +3814,9 @@
       <c r="H96" t="n">
         <v>0</v>
       </c>
+      <c r="I96" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -3558,6 +3849,9 @@
       <c r="H97" t="n">
         <v>0</v>
       </c>
+      <c r="I97" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -3590,6 +3884,9 @@
       <c r="H98" t="n">
         <v>0</v>
       </c>
+      <c r="I98" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -3622,6 +3919,9 @@
       <c r="H99" t="n">
         <v>0</v>
       </c>
+      <c r="I99" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -3649,10 +3949,13 @@
         <v>0</v>
       </c>
       <c r="G100" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H100" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I100" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="101">
@@ -3681,10 +3984,13 @@
         <v>0</v>
       </c>
       <c r="G101" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H101" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I101" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="102">
@@ -3718,6 +4024,9 @@
       <c r="H102" t="n">
         <v>0</v>
       </c>
+      <c r="I102" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -3745,10 +4054,13 @@
         <v>0</v>
       </c>
       <c r="G103" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H103" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I103" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="104">
@@ -3777,10 +4089,13 @@
         <v>0</v>
       </c>
       <c r="G104" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H104" t="n">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="I104" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="105">
@@ -3809,10 +4124,13 @@
         <v>0</v>
       </c>
       <c r="G105" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H105" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I105" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="106">
@@ -3841,10 +4159,13 @@
         <v>0</v>
       </c>
       <c r="G106" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H106" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I106" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="107">
@@ -3878,6 +4199,9 @@
       <c r="H107" t="n">
         <v>0</v>
       </c>
+      <c r="I107" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -3905,10 +4229,13 @@
         <v>0</v>
       </c>
       <c r="G108" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H108" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I108" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="109">
@@ -3940,6 +4267,9 @@
         <v>0</v>
       </c>
       <c r="H109" t="n">
+        <v>0</v>
+      </c>
+      <c r="I109" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Daily IST report: add CSV/MD/XLSX (#393)
Co-authored-by: codethesept <198977775+codethesept@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/reports/submissions_daily_matrix.xlsx
+++ b/reports/submissions_daily_matrix.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I109"/>
+  <dimension ref="A1:J109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,8 +442,9 @@
     <col width="12" customWidth="1" min="5" max="5"/>
     <col width="12" customWidth="1" min="6" max="6"/>
     <col width="12" customWidth="1" min="7" max="7"/>
-    <col width="13" customWidth="1" min="8" max="8"/>
+    <col width="12" customWidth="1" min="8" max="8"/>
     <col width="13" customWidth="1" min="9" max="9"/>
+    <col width="13" customWidth="1" min="10" max="10"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -482,12 +483,17 @@
           <t>2026-02-18</t>
         </is>
       </c>
-      <c r="H1" s="2" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>2026-02-19</t>
+        </is>
+      </c>
+      <c r="I1" s="2" t="inlineStr">
         <is>
           <t>total_files</t>
         </is>
       </c>
-      <c r="I1" s="2" t="inlineStr">
+      <c r="J1" s="2" t="inlineStr">
         <is>
           <t>unique_days</t>
         </is>
@@ -525,7 +531,10 @@
         <v>1</v>
       </c>
       <c r="I2" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="J2" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -557,9 +566,12 @@
         <v>1</v>
       </c>
       <c r="H3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" t="n">
         <v>1</v>
       </c>
     </row>
@@ -592,10 +604,13 @@
         <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="J4" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -630,7 +645,10 @@
         <v>1</v>
       </c>
       <c r="I5" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="J5" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="6">
@@ -667,6 +685,9 @@
       <c r="I6" t="n">
         <v>0</v>
       </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -700,7 +721,10 @@
         <v>1</v>
       </c>
       <c r="I7" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="J7" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="8">
@@ -735,7 +759,10 @@
         <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="J8" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="9">
@@ -770,7 +797,10 @@
         <v>1</v>
       </c>
       <c r="I9" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="J9" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="10">
@@ -805,7 +835,10 @@
         <v>1</v>
       </c>
       <c r="I10" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="J10" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="11">
@@ -837,10 +870,13 @@
         <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="J11" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -875,7 +911,10 @@
         <v>1</v>
       </c>
       <c r="I12" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="J12" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="13">
@@ -910,7 +949,10 @@
         <v>1</v>
       </c>
       <c r="I13" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="J13" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="14">
@@ -945,7 +987,10 @@
         <v>1</v>
       </c>
       <c r="I14" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="J14" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="15">
@@ -977,9 +1022,12 @@
         <v>0</v>
       </c>
       <c r="H15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I15" t="n">
+        <v>1</v>
+      </c>
+      <c r="J15" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1017,6 +1065,9 @@
       <c r="I16" t="n">
         <v>0</v>
       </c>
+      <c r="J16" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1050,7 +1101,10 @@
         <v>1</v>
       </c>
       <c r="I17" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="J17" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="18">
@@ -1085,7 +1139,10 @@
         <v>1</v>
       </c>
       <c r="I18" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="J18" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="19">
@@ -1120,7 +1177,10 @@
         <v>1</v>
       </c>
       <c r="I19" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="J19" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="20">
@@ -1152,9 +1212,12 @@
         <v>1</v>
       </c>
       <c r="H20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I20" t="n">
+        <v>1</v>
+      </c>
+      <c r="J20" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1192,6 +1255,9 @@
       <c r="I21" t="n">
         <v>0</v>
       </c>
+      <c r="J21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1227,6 +1293,9 @@
       <c r="I22" t="n">
         <v>0</v>
       </c>
+      <c r="J22" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1262,6 +1331,9 @@
       <c r="I23" t="n">
         <v>0</v>
       </c>
+      <c r="J23" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1292,9 +1364,12 @@
         <v>1</v>
       </c>
       <c r="H24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I24" t="n">
+        <v>1</v>
+      </c>
+      <c r="J24" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1330,7 +1405,10 @@
         <v>1</v>
       </c>
       <c r="I25" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="J25" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="26">
@@ -1367,6 +1445,9 @@
       <c r="I26" t="n">
         <v>0</v>
       </c>
+      <c r="J26" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1397,9 +1478,12 @@
         <v>3</v>
       </c>
       <c r="H27" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" t="n">
         <v>3</v>
       </c>
-      <c r="I27" t="n">
+      <c r="J27" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1437,6 +1521,9 @@
       <c r="I28" t="n">
         <v>0</v>
       </c>
+      <c r="J28" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1472,6 +1559,9 @@
       <c r="I29" t="n">
         <v>0</v>
       </c>
+      <c r="J29" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1507,6 +1597,9 @@
       <c r="I30" t="n">
         <v>0</v>
       </c>
+      <c r="J30" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1540,7 +1633,10 @@
         <v>1</v>
       </c>
       <c r="I31" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="J31" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="32">
@@ -1575,7 +1671,10 @@
         <v>1</v>
       </c>
       <c r="I32" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="J32" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="33">
@@ -1610,7 +1709,10 @@
         <v>1</v>
       </c>
       <c r="I33" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="J33" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="34">
@@ -1645,7 +1747,10 @@
         <v>1</v>
       </c>
       <c r="I34" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="J34" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="35">
@@ -1680,7 +1785,10 @@
         <v>1</v>
       </c>
       <c r="I35" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="J35" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="36">
@@ -1712,10 +1820,13 @@
         <v>0</v>
       </c>
       <c r="H36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I36" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="J36" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="37">
@@ -1747,9 +1858,12 @@
         <v>1</v>
       </c>
       <c r="H37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I37" t="n">
+        <v>1</v>
+      </c>
+      <c r="J37" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1787,6 +1901,9 @@
       <c r="I38" t="n">
         <v>0</v>
       </c>
+      <c r="J38" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1822,6 +1939,9 @@
       <c r="I39" t="n">
         <v>0</v>
       </c>
+      <c r="J39" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1855,7 +1975,10 @@
         <v>1</v>
       </c>
       <c r="I40" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="J40" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="41">
@@ -1890,7 +2013,10 @@
         <v>1</v>
       </c>
       <c r="I41" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="J41" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="42">
@@ -1925,7 +2051,10 @@
         <v>1</v>
       </c>
       <c r="I42" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="J42" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="43">
@@ -1957,9 +2086,12 @@
         <v>21</v>
       </c>
       <c r="H43" t="n">
+        <v>0</v>
+      </c>
+      <c r="I43" t="n">
         <v>21</v>
       </c>
-      <c r="I43" t="n">
+      <c r="J43" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1997,6 +2129,9 @@
       <c r="I44" t="n">
         <v>0</v>
       </c>
+      <c r="J44" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -2027,9 +2162,12 @@
         <v>1</v>
       </c>
       <c r="H45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I45" t="n">
+        <v>1</v>
+      </c>
+      <c r="J45" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2065,7 +2203,10 @@
         <v>1</v>
       </c>
       <c r="I46" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="J46" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="47">
@@ -2100,7 +2241,10 @@
         <v>1</v>
       </c>
       <c r="I47" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="J47" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="48">
@@ -2137,6 +2281,9 @@
       <c r="I48" t="n">
         <v>0</v>
       </c>
+      <c r="J48" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2170,7 +2317,10 @@
         <v>1</v>
       </c>
       <c r="I49" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="J49" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="50">
@@ -2202,10 +2352,13 @@
         <v>0</v>
       </c>
       <c r="H50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I50" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="J50" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="51">
@@ -2242,6 +2395,9 @@
       <c r="I51" t="n">
         <v>0</v>
       </c>
+      <c r="J51" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -2275,7 +2431,10 @@
         <v>1</v>
       </c>
       <c r="I52" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="J52" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="53">
@@ -2307,10 +2466,13 @@
         <v>0</v>
       </c>
       <c r="H53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I53" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="J53" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="54">
@@ -2347,6 +2509,9 @@
       <c r="I54" t="n">
         <v>0</v>
       </c>
+      <c r="J54" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -2380,7 +2545,10 @@
         <v>1</v>
       </c>
       <c r="I55" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="J55" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="56">
@@ -2417,6 +2585,9 @@
       <c r="I56" t="n">
         <v>0</v>
       </c>
+      <c r="J56" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -2447,10 +2618,13 @@
         <v>0</v>
       </c>
       <c r="H57" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I57" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="J57" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="58">
@@ -2482,9 +2656,12 @@
         <v>1</v>
       </c>
       <c r="H58" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I58" t="n">
+        <v>1</v>
+      </c>
+      <c r="J58" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2517,10 +2694,13 @@
         <v>0</v>
       </c>
       <c r="H59" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I59" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="J59" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="60">
@@ -2555,7 +2735,10 @@
         <v>1</v>
       </c>
       <c r="I60" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="J60" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="61">
@@ -2587,9 +2770,12 @@
         <v>1</v>
       </c>
       <c r="H61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I61" t="n">
+        <v>1</v>
+      </c>
+      <c r="J61" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2627,6 +2813,9 @@
       <c r="I62" t="n">
         <v>0</v>
       </c>
+      <c r="J62" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -2662,6 +2851,9 @@
       <c r="I63" t="n">
         <v>0</v>
       </c>
+      <c r="J63" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2695,7 +2887,10 @@
         <v>1</v>
       </c>
       <c r="I64" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="J64" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="65">
@@ -2732,6 +2927,9 @@
       <c r="I65" t="n">
         <v>0</v>
       </c>
+      <c r="J65" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -2767,6 +2965,9 @@
       <c r="I66" t="n">
         <v>0</v>
       </c>
+      <c r="J66" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -2802,6 +3003,9 @@
       <c r="I67" t="n">
         <v>0</v>
       </c>
+      <c r="J67" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -2837,6 +3041,9 @@
       <c r="I68" t="n">
         <v>0</v>
       </c>
+      <c r="J68" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -2872,6 +3079,9 @@
       <c r="I69" t="n">
         <v>0</v>
       </c>
+      <c r="J69" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -2905,7 +3115,10 @@
         <v>1</v>
       </c>
       <c r="I70" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="J70" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="71">
@@ -2942,6 +3155,9 @@
       <c r="I71" t="n">
         <v>0</v>
       </c>
+      <c r="J71" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -2977,6 +3193,9 @@
       <c r="I72" t="n">
         <v>0</v>
       </c>
+      <c r="J72" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -3012,6 +3231,9 @@
       <c r="I73" t="n">
         <v>0</v>
       </c>
+      <c r="J73" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -3042,10 +3264,13 @@
         <v>13</v>
       </c>
       <c r="H74" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="I74" t="n">
-        <v>1</v>
+        <v>14</v>
+      </c>
+      <c r="J74" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="75">
@@ -3082,6 +3307,9 @@
       <c r="I75" t="n">
         <v>0</v>
       </c>
+      <c r="J75" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -3112,9 +3340,12 @@
         <v>1</v>
       </c>
       <c r="H76" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I76" t="n">
+        <v>1</v>
+      </c>
+      <c r="J76" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3152,6 +3383,9 @@
       <c r="I77" t="n">
         <v>0</v>
       </c>
+      <c r="J77" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -3187,6 +3421,9 @@
       <c r="I78" t="n">
         <v>0</v>
       </c>
+      <c r="J78" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -3222,6 +3459,9 @@
       <c r="I79" t="n">
         <v>0</v>
       </c>
+      <c r="J79" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -3252,10 +3492,13 @@
         <v>0</v>
       </c>
       <c r="H80" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I80" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="J80" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="81">
@@ -3287,10 +3530,13 @@
         <v>0</v>
       </c>
       <c r="H81" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I81" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="J81" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="82">
@@ -3325,7 +3571,10 @@
         <v>1</v>
       </c>
       <c r="I82" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="J82" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="83">
@@ -3362,6 +3611,9 @@
       <c r="I83" t="n">
         <v>0</v>
       </c>
+      <c r="J83" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -3392,9 +3644,12 @@
         <v>1</v>
       </c>
       <c r="H84" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I84" t="n">
+        <v>1</v>
+      </c>
+      <c r="J84" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3432,6 +3687,9 @@
       <c r="I85" t="n">
         <v>0</v>
       </c>
+      <c r="J85" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -3462,9 +3720,12 @@
         <v>1</v>
       </c>
       <c r="H86" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I86" t="n">
+        <v>1</v>
+      </c>
+      <c r="J86" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3502,6 +3763,9 @@
       <c r="I87" t="n">
         <v>0</v>
       </c>
+      <c r="J87" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -3532,10 +3796,13 @@
         <v>0</v>
       </c>
       <c r="H88" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I88" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="J88" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="89">
@@ -3572,6 +3839,9 @@
       <c r="I89" t="n">
         <v>0</v>
       </c>
+      <c r="J89" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -3607,6 +3877,9 @@
       <c r="I90" t="n">
         <v>0</v>
       </c>
+      <c r="J90" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -3642,6 +3915,9 @@
       <c r="I91" t="n">
         <v>0</v>
       </c>
+      <c r="J91" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -3677,6 +3953,9 @@
       <c r="I92" t="n">
         <v>0</v>
       </c>
+      <c r="J92" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -3712,6 +3991,9 @@
       <c r="I93" t="n">
         <v>0</v>
       </c>
+      <c r="J93" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -3742,10 +4024,13 @@
         <v>0</v>
       </c>
       <c r="H94" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I94" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="J94" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="95">
@@ -3777,10 +4062,13 @@
         <v>30</v>
       </c>
       <c r="H95" t="n">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="I95" t="n">
-        <v>1</v>
+        <v>31</v>
+      </c>
+      <c r="J95" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="96">
@@ -3817,6 +4105,9 @@
       <c r="I96" t="n">
         <v>0</v>
       </c>
+      <c r="J96" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -3852,6 +4143,9 @@
       <c r="I97" t="n">
         <v>0</v>
       </c>
+      <c r="J97" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -3887,6 +4181,9 @@
       <c r="I98" t="n">
         <v>0</v>
       </c>
+      <c r="J98" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -3922,6 +4219,9 @@
       <c r="I99" t="n">
         <v>0</v>
       </c>
+      <c r="J99" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -3952,9 +4252,12 @@
         <v>1</v>
       </c>
       <c r="H100" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I100" t="n">
+        <v>1</v>
+      </c>
+      <c r="J100" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3990,7 +4293,10 @@
         <v>1</v>
       </c>
       <c r="I101" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="J101" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="102">
@@ -4027,6 +4333,9 @@
       <c r="I102" t="n">
         <v>0</v>
       </c>
+      <c r="J102" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -4060,7 +4369,10 @@
         <v>1</v>
       </c>
       <c r="I103" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="J103" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="104">
@@ -4092,9 +4404,12 @@
         <v>12</v>
       </c>
       <c r="H104" t="n">
+        <v>0</v>
+      </c>
+      <c r="I104" t="n">
         <v>12</v>
       </c>
-      <c r="I104" t="n">
+      <c r="J104" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4130,7 +4445,10 @@
         <v>1</v>
       </c>
       <c r="I105" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="J105" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="106">
@@ -4165,7 +4483,10 @@
         <v>1</v>
       </c>
       <c r="I106" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="J106" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="107">
@@ -4202,6 +4523,9 @@
       <c r="I107" t="n">
         <v>0</v>
       </c>
+      <c r="J107" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -4232,9 +4556,12 @@
         <v>1</v>
       </c>
       <c r="H108" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I108" t="n">
+        <v>1</v>
+      </c>
+      <c r="J108" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4270,6 +4597,9 @@
         <v>0</v>
       </c>
       <c r="I109" t="n">
+        <v>0</v>
+      </c>
+      <c r="J109" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Daily IST report: add CSV/MD/XLSX (#467)
Co-authored-by: codethesept <198977775+codethesept@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/reports/submissions_daily_matrix.xlsx
+++ b/reports/submissions_daily_matrix.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J109"/>
+  <dimension ref="A1:K109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,8 +443,9 @@
     <col width="12" customWidth="1" min="6" max="6"/>
     <col width="12" customWidth="1" min="7" max="7"/>
     <col width="12" customWidth="1" min="8" max="8"/>
-    <col width="13" customWidth="1" min="9" max="9"/>
+    <col width="12" customWidth="1" min="9" max="9"/>
     <col width="13" customWidth="1" min="10" max="10"/>
+    <col width="13" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -488,12 +489,17 @@
           <t>2026-02-19</t>
         </is>
       </c>
-      <c r="I1" s="2" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>2026-02-23</t>
+        </is>
+      </c>
+      <c r="J1" s="2" t="inlineStr">
         <is>
           <t>total_files</t>
         </is>
       </c>
-      <c r="J1" s="2" t="inlineStr">
+      <c r="K1" s="2" t="inlineStr">
         <is>
           <t>unique_days</t>
         </is>
@@ -531,10 +537,13 @@
         <v>1</v>
       </c>
       <c r="I2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J2" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="K2" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="3">
@@ -572,7 +581,10 @@
         <v>1</v>
       </c>
       <c r="J3" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="K3" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -610,7 +622,10 @@
         <v>1</v>
       </c>
       <c r="J4" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="K4" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="5">
@@ -645,10 +660,13 @@
         <v>1</v>
       </c>
       <c r="I5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J5" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="K5" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="6">
@@ -683,10 +701,13 @@
         <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="K6" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -721,10 +742,13 @@
         <v>1</v>
       </c>
       <c r="I7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J7" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="K7" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="8">
@@ -759,10 +783,13 @@
         <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J8" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="K8" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="9">
@@ -797,10 +824,13 @@
         <v>1</v>
       </c>
       <c r="I9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="K9" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="10">
@@ -835,11 +865,14 @@
         <v>1</v>
       </c>
       <c r="I10" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J10" t="n">
         <v>2</v>
       </c>
+      <c r="K10" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -876,7 +909,10 @@
         <v>1</v>
       </c>
       <c r="J11" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="K11" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="12">
@@ -911,10 +947,13 @@
         <v>1</v>
       </c>
       <c r="I12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J12" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="K12" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="13">
@@ -949,11 +988,14 @@
         <v>1</v>
       </c>
       <c r="I13" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J13" t="n">
         <v>2</v>
       </c>
+      <c r="K13" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -987,10 +1029,13 @@
         <v>1</v>
       </c>
       <c r="I14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J14" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="K14" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="15">
@@ -1028,7 +1073,10 @@
         <v>1</v>
       </c>
       <c r="J15" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="K15" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="16">
@@ -1063,10 +1111,13 @@
         <v>0</v>
       </c>
       <c r="I16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="K16" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="17">
@@ -1101,10 +1152,13 @@
         <v>1</v>
       </c>
       <c r="I17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J17" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="K17" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="18">
@@ -1139,10 +1193,13 @@
         <v>1</v>
       </c>
       <c r="I18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J18" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="K18" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="19">
@@ -1177,11 +1234,14 @@
         <v>1</v>
       </c>
       <c r="I19" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J19" t="n">
         <v>2</v>
       </c>
+      <c r="K19" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1218,7 +1278,10 @@
         <v>1</v>
       </c>
       <c r="J20" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="K20" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="21">
@@ -1258,6 +1321,9 @@
       <c r="J21" t="n">
         <v>0</v>
       </c>
+      <c r="K21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1296,6 +1362,9 @@
       <c r="J22" t="n">
         <v>0</v>
       </c>
+      <c r="K22" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1334,6 +1403,9 @@
       <c r="J23" t="n">
         <v>0</v>
       </c>
+      <c r="K23" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1370,7 +1442,10 @@
         <v>1</v>
       </c>
       <c r="J24" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="K24" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="25">
@@ -1405,10 +1480,13 @@
         <v>1</v>
       </c>
       <c r="I25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J25" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="K25" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="26">
@@ -1448,6 +1526,9 @@
       <c r="J26" t="n">
         <v>0</v>
       </c>
+      <c r="K26" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1481,10 +1562,13 @@
         <v>0</v>
       </c>
       <c r="I27" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J27" t="n">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="K27" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="28">
@@ -1524,6 +1608,9 @@
       <c r="J28" t="n">
         <v>0</v>
       </c>
+      <c r="K28" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1562,6 +1649,9 @@
       <c r="J29" t="n">
         <v>0</v>
       </c>
+      <c r="K29" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1600,6 +1690,9 @@
       <c r="J30" t="n">
         <v>0</v>
       </c>
+      <c r="K30" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1633,10 +1726,13 @@
         <v>1</v>
       </c>
       <c r="I31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J31" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="K31" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="32">
@@ -1671,10 +1767,13 @@
         <v>1</v>
       </c>
       <c r="I32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J32" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="K32" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="33">
@@ -1709,10 +1808,13 @@
         <v>1</v>
       </c>
       <c r="I33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J33" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="K33" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="34">
@@ -1747,10 +1849,13 @@
         <v>1</v>
       </c>
       <c r="I34" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J34" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="K34" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="35">
@@ -1785,10 +1890,13 @@
         <v>1</v>
       </c>
       <c r="I35" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J35" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="K35" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="36">
@@ -1826,7 +1934,10 @@
         <v>1</v>
       </c>
       <c r="J36" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="K36" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="37">
@@ -1861,9 +1972,12 @@
         <v>0</v>
       </c>
       <c r="I37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J37" t="n">
+        <v>1</v>
+      </c>
+      <c r="K37" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1904,6 +2018,9 @@
       <c r="J38" t="n">
         <v>0</v>
       </c>
+      <c r="K38" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1942,6 +2059,9 @@
       <c r="J39" t="n">
         <v>0</v>
       </c>
+      <c r="K39" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1975,10 +2095,13 @@
         <v>1</v>
       </c>
       <c r="I40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J40" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="K40" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="41">
@@ -2013,10 +2136,13 @@
         <v>1</v>
       </c>
       <c r="I41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J41" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="K41" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="42">
@@ -2051,10 +2177,13 @@
         <v>1</v>
       </c>
       <c r="I42" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J42" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="K42" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="43">
@@ -2089,9 +2218,12 @@
         <v>0</v>
       </c>
       <c r="I43" t="n">
+        <v>0</v>
+      </c>
+      <c r="J43" t="n">
         <v>21</v>
       </c>
-      <c r="J43" t="n">
+      <c r="K43" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2132,6 +2264,9 @@
       <c r="J44" t="n">
         <v>0</v>
       </c>
+      <c r="K44" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -2168,7 +2303,10 @@
         <v>1</v>
       </c>
       <c r="J45" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="K45" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="46">
@@ -2203,10 +2341,13 @@
         <v>1</v>
       </c>
       <c r="I46" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J46" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="K46" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="47">
@@ -2241,10 +2382,13 @@
         <v>1</v>
       </c>
       <c r="I47" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J47" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="K47" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="48">
@@ -2284,6 +2428,9 @@
       <c r="J48" t="n">
         <v>0</v>
       </c>
+      <c r="K48" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2317,10 +2464,13 @@
         <v>1</v>
       </c>
       <c r="I49" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J49" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="K49" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="50">
@@ -2358,7 +2508,10 @@
         <v>1</v>
       </c>
       <c r="J50" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="K50" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="51">
@@ -2398,6 +2551,9 @@
       <c r="J51" t="n">
         <v>0</v>
       </c>
+      <c r="K51" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -2431,11 +2587,14 @@
         <v>1</v>
       </c>
       <c r="I52" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J52" t="n">
         <v>2</v>
       </c>
+      <c r="K52" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -2472,7 +2631,10 @@
         <v>1</v>
       </c>
       <c r="J53" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="K53" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="54">
@@ -2512,6 +2674,9 @@
       <c r="J54" t="n">
         <v>0</v>
       </c>
+      <c r="K54" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -2545,10 +2710,13 @@
         <v>1</v>
       </c>
       <c r="I55" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J55" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="K55" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="56">
@@ -2588,6 +2756,9 @@
       <c r="J56" t="n">
         <v>0</v>
       </c>
+      <c r="K56" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -2624,7 +2795,10 @@
         <v>1</v>
       </c>
       <c r="J57" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="K57" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="58">
@@ -2662,7 +2836,10 @@
         <v>1</v>
       </c>
       <c r="J58" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="K58" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="59">
@@ -2700,7 +2877,10 @@
         <v>1</v>
       </c>
       <c r="J59" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="K59" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="60">
@@ -2735,10 +2915,13 @@
         <v>1</v>
       </c>
       <c r="I60" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J60" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="K60" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="61">
@@ -2773,9 +2956,12 @@
         <v>0</v>
       </c>
       <c r="I61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J61" t="n">
+        <v>1</v>
+      </c>
+      <c r="K61" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2816,6 +3002,9 @@
       <c r="J62" t="n">
         <v>0</v>
       </c>
+      <c r="K62" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -2854,6 +3043,9 @@
       <c r="J63" t="n">
         <v>0</v>
       </c>
+      <c r="K63" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2887,10 +3079,13 @@
         <v>1</v>
       </c>
       <c r="I64" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J64" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="K64" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="65">
@@ -2930,6 +3125,9 @@
       <c r="J65" t="n">
         <v>0</v>
       </c>
+      <c r="K65" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -2968,6 +3166,9 @@
       <c r="J66" t="n">
         <v>0</v>
       </c>
+      <c r="K66" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -3001,10 +3202,13 @@
         <v>0</v>
       </c>
       <c r="I67" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J67" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="K67" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="68">
@@ -3044,6 +3248,9 @@
       <c r="J68" t="n">
         <v>0</v>
       </c>
+      <c r="K68" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -3082,6 +3289,9 @@
       <c r="J69" t="n">
         <v>0</v>
       </c>
+      <c r="K69" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -3115,10 +3325,13 @@
         <v>1</v>
       </c>
       <c r="I70" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J70" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="K70" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="71">
@@ -3153,10 +3366,13 @@
         <v>0</v>
       </c>
       <c r="I71" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J71" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="K71" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="72">
@@ -3196,6 +3412,9 @@
       <c r="J72" t="n">
         <v>0</v>
       </c>
+      <c r="K72" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -3234,6 +3453,9 @@
       <c r="J73" t="n">
         <v>0</v>
       </c>
+      <c r="K73" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -3267,10 +3489,13 @@
         <v>1</v>
       </c>
       <c r="I74" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="J74" t="n">
-        <v>2</v>
+        <v>15</v>
+      </c>
+      <c r="K74" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="75">
@@ -3310,6 +3535,9 @@
       <c r="J75" t="n">
         <v>0</v>
       </c>
+      <c r="K75" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -3346,7 +3574,10 @@
         <v>1</v>
       </c>
       <c r="J76" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="K76" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="77">
@@ -3386,6 +3617,9 @@
       <c r="J77" t="n">
         <v>0</v>
       </c>
+      <c r="K77" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -3424,6 +3658,9 @@
       <c r="J78" t="n">
         <v>0</v>
       </c>
+      <c r="K78" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -3457,10 +3694,13 @@
         <v>0</v>
       </c>
       <c r="I79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J79" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="K79" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="80">
@@ -3498,7 +3738,10 @@
         <v>1</v>
       </c>
       <c r="J80" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="K80" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="81">
@@ -3536,7 +3779,10 @@
         <v>1</v>
       </c>
       <c r="J81" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="K81" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="82">
@@ -3571,10 +3817,13 @@
         <v>1</v>
       </c>
       <c r="I82" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J82" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="K82" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="83">
@@ -3614,6 +3863,9 @@
       <c r="J83" t="n">
         <v>0</v>
       </c>
+      <c r="K83" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -3647,9 +3899,12 @@
         <v>0</v>
       </c>
       <c r="I84" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J84" t="n">
+        <v>1</v>
+      </c>
+      <c r="K84" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3690,6 +3945,9 @@
       <c r="J85" t="n">
         <v>0</v>
       </c>
+      <c r="K85" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -3726,7 +3984,10 @@
         <v>1</v>
       </c>
       <c r="J86" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="K86" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="87">
@@ -3766,6 +4027,9 @@
       <c r="J87" t="n">
         <v>0</v>
       </c>
+      <c r="K87" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -3802,7 +4066,10 @@
         <v>1</v>
       </c>
       <c r="J88" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="K88" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="89">
@@ -3842,6 +4109,9 @@
       <c r="J89" t="n">
         <v>0</v>
       </c>
+      <c r="K89" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -3875,10 +4145,13 @@
         <v>0</v>
       </c>
       <c r="I90" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J90" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="K90" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="91">
@@ -3918,6 +4191,9 @@
       <c r="J91" t="n">
         <v>0</v>
       </c>
+      <c r="K91" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -3956,6 +4232,9 @@
       <c r="J92" t="n">
         <v>0</v>
       </c>
+      <c r="K92" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -3989,10 +4268,13 @@
         <v>0</v>
       </c>
       <c r="I93" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J93" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="K93" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="94">
@@ -4030,7 +4312,10 @@
         <v>1</v>
       </c>
       <c r="J94" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="K94" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="95">
@@ -4065,10 +4350,13 @@
         <v>1</v>
       </c>
       <c r="I95" t="n">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="J95" t="n">
-        <v>2</v>
+        <v>32</v>
+      </c>
+      <c r="K95" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="96">
@@ -4108,6 +4396,9 @@
       <c r="J96" t="n">
         <v>0</v>
       </c>
+      <c r="K96" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -4146,6 +4437,9 @@
       <c r="J97" t="n">
         <v>0</v>
       </c>
+      <c r="K97" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -4184,6 +4478,9 @@
       <c r="J98" t="n">
         <v>0</v>
       </c>
+      <c r="K98" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -4222,6 +4519,9 @@
       <c r="J99" t="n">
         <v>0</v>
       </c>
+      <c r="K99" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -4255,9 +4555,12 @@
         <v>0</v>
       </c>
       <c r="I100" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J100" t="n">
+        <v>1</v>
+      </c>
+      <c r="K100" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4293,10 +4596,13 @@
         <v>1</v>
       </c>
       <c r="I101" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J101" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="K101" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="102">
@@ -4336,6 +4642,9 @@
       <c r="J102" t="n">
         <v>0</v>
       </c>
+      <c r="K102" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -4369,10 +4678,13 @@
         <v>1</v>
       </c>
       <c r="I103" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J103" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="K103" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="104">
@@ -4407,9 +4719,12 @@
         <v>0</v>
       </c>
       <c r="I104" t="n">
+        <v>0</v>
+      </c>
+      <c r="J104" t="n">
         <v>12</v>
       </c>
-      <c r="J104" t="n">
+      <c r="K104" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4445,10 +4760,13 @@
         <v>1</v>
       </c>
       <c r="I105" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J105" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="K105" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="106">
@@ -4483,10 +4801,13 @@
         <v>1</v>
       </c>
       <c r="I106" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J106" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="K106" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="107">
@@ -4526,6 +4847,9 @@
       <c r="J107" t="n">
         <v>0</v>
       </c>
+      <c r="K107" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -4562,7 +4886,10 @@
         <v>1</v>
       </c>
       <c r="J108" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="K108" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="109">
@@ -4600,6 +4927,9 @@
         <v>0</v>
       </c>
       <c r="J109" t="n">
+        <v>0</v>
+      </c>
+      <c r="K109" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Daily IST report: add CSV/MD/XLSX (#749)
Co-authored-by: codethesept <198977775+codethesept@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/reports/submissions_daily_matrix.xlsx
+++ b/reports/submissions_daily_matrix.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K109"/>
+  <dimension ref="A1:L109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,8 +444,9 @@
     <col width="12" customWidth="1" min="7" max="7"/>
     <col width="12" customWidth="1" min="8" max="8"/>
     <col width="12" customWidth="1" min="9" max="9"/>
-    <col width="13" customWidth="1" min="10" max="10"/>
+    <col width="12" customWidth="1" min="10" max="10"/>
     <col width="13" customWidth="1" min="11" max="11"/>
+    <col width="13" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -494,12 +495,17 @@
           <t>2026-02-23</t>
         </is>
       </c>
-      <c r="J1" s="2" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>2026-02-24</t>
+        </is>
+      </c>
+      <c r="K1" s="2" t="inlineStr">
         <is>
           <t>total_files</t>
         </is>
       </c>
-      <c r="K1" s="2" t="inlineStr">
+      <c r="L1" s="2" t="inlineStr">
         <is>
           <t>unique_days</t>
         </is>
@@ -540,11 +546,14 @@
         <v>1</v>
       </c>
       <c r="J2" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K2" t="n">
         <v>3</v>
       </c>
+      <c r="L2" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -581,11 +590,14 @@
         <v>1</v>
       </c>
       <c r="J3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
         <v>2</v>
       </c>
+      <c r="L3" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -622,10 +634,13 @@
         <v>1</v>
       </c>
       <c r="J4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K4" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="L4" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="5">
@@ -663,10 +678,13 @@
         <v>1</v>
       </c>
       <c r="J5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K5" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="L5" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="6">
@@ -707,7 +725,10 @@
         <v>1</v>
       </c>
       <c r="K6" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="L6" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="7">
@@ -745,10 +766,13 @@
         <v>1</v>
       </c>
       <c r="J7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K7" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="L7" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="8">
@@ -786,10 +810,13 @@
         <v>1</v>
       </c>
       <c r="J8" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K8" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="L8" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="9">
@@ -827,10 +854,13 @@
         <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K9" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="L9" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="10">
@@ -868,10 +898,13 @@
         <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K10" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="L10" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="11">
@@ -909,10 +942,13 @@
         <v>1</v>
       </c>
       <c r="J11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K11" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="L11" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="12">
@@ -950,10 +986,13 @@
         <v>1</v>
       </c>
       <c r="J12" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K12" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="L12" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="13">
@@ -991,10 +1030,13 @@
         <v>0</v>
       </c>
       <c r="J13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K13" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="L13" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="14">
@@ -1032,10 +1074,13 @@
         <v>1</v>
       </c>
       <c r="J14" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K14" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="L14" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="15">
@@ -1073,11 +1118,14 @@
         <v>1</v>
       </c>
       <c r="J15" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K15" t="n">
         <v>2</v>
       </c>
+      <c r="L15" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1117,7 +1165,10 @@
         <v>1</v>
       </c>
       <c r="K16" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="L16" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="17">
@@ -1155,10 +1206,13 @@
         <v>1</v>
       </c>
       <c r="J17" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K17" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="L17" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="18">
@@ -1196,10 +1250,13 @@
         <v>1</v>
       </c>
       <c r="J18" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K18" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="L18" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="19">
@@ -1237,10 +1294,13 @@
         <v>0</v>
       </c>
       <c r="J19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K19" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="L19" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="20">
@@ -1278,10 +1338,13 @@
         <v>1</v>
       </c>
       <c r="J20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K20" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="L20" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="21">
@@ -1324,6 +1387,9 @@
       <c r="K21" t="n">
         <v>0</v>
       </c>
+      <c r="L21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1365,6 +1431,9 @@
       <c r="K22" t="n">
         <v>0</v>
       </c>
+      <c r="L22" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1406,6 +1475,9 @@
       <c r="K23" t="n">
         <v>0</v>
       </c>
+      <c r="L23" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1442,10 +1514,13 @@
         <v>1</v>
       </c>
       <c r="J24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K24" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="L24" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="25">
@@ -1483,11 +1558,14 @@
         <v>1</v>
       </c>
       <c r="J25" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K25" t="n">
         <v>3</v>
       </c>
+      <c r="L25" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1524,10 +1602,13 @@
         <v>0</v>
       </c>
       <c r="J26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K26" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="L26" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="27">
@@ -1565,10 +1646,13 @@
         <v>1</v>
       </c>
       <c r="J27" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K27" t="n">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="L27" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="28">
@@ -1611,6 +1695,9 @@
       <c r="K28" t="n">
         <v>0</v>
       </c>
+      <c r="L28" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1652,6 +1739,9 @@
       <c r="K29" t="n">
         <v>0</v>
       </c>
+      <c r="L29" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1693,6 +1783,9 @@
       <c r="K30" t="n">
         <v>0</v>
       </c>
+      <c r="L30" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1729,10 +1822,13 @@
         <v>1</v>
       </c>
       <c r="J31" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K31" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="L31" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="32">
@@ -1770,10 +1866,13 @@
         <v>1</v>
       </c>
       <c r="J32" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K32" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="L32" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="33">
@@ -1811,10 +1910,13 @@
         <v>1</v>
       </c>
       <c r="J33" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K33" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="L33" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="34">
@@ -1852,10 +1954,13 @@
         <v>1</v>
       </c>
       <c r="J34" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K34" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="L34" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="35">
@@ -1893,10 +1998,13 @@
         <v>1</v>
       </c>
       <c r="J35" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K35" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="L35" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="36">
@@ -1934,10 +2042,13 @@
         <v>1</v>
       </c>
       <c r="J36" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K36" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="L36" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="37">
@@ -1978,7 +2089,10 @@
         <v>1</v>
       </c>
       <c r="K37" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="L37" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="38">
@@ -2021,6 +2135,9 @@
       <c r="K38" t="n">
         <v>0</v>
       </c>
+      <c r="L38" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -2062,6 +2179,9 @@
       <c r="K39" t="n">
         <v>0</v>
       </c>
+      <c r="L39" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -2098,10 +2218,13 @@
         <v>1</v>
       </c>
       <c r="J40" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K40" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="L40" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="41">
@@ -2139,10 +2262,13 @@
         <v>1</v>
       </c>
       <c r="J41" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K41" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="L41" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="42">
@@ -2180,10 +2306,13 @@
         <v>1</v>
       </c>
       <c r="J42" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K42" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="L42" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="43">
@@ -2221,9 +2350,12 @@
         <v>0</v>
       </c>
       <c r="J43" t="n">
+        <v>0</v>
+      </c>
+      <c r="K43" t="n">
         <v>21</v>
       </c>
-      <c r="K43" t="n">
+      <c r="L43" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2262,10 +2394,13 @@
         <v>0</v>
       </c>
       <c r="J44" t="n">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="K44" t="n">
-        <v>0</v>
+        <v>42</v>
+      </c>
+      <c r="L44" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="45">
@@ -2303,11 +2438,14 @@
         <v>1</v>
       </c>
       <c r="J45" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K45" t="n">
         <v>2</v>
       </c>
+      <c r="L45" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2344,10 +2482,13 @@
         <v>1</v>
       </c>
       <c r="J46" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K46" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="L46" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="47">
@@ -2385,10 +2526,13 @@
         <v>1</v>
       </c>
       <c r="J47" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K47" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="L47" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="48">
@@ -2431,6 +2575,9 @@
       <c r="K48" t="n">
         <v>0</v>
       </c>
+      <c r="L48" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2467,10 +2614,13 @@
         <v>1</v>
       </c>
       <c r="J49" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K49" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="L49" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="50">
@@ -2508,10 +2658,13 @@
         <v>1</v>
       </c>
       <c r="J50" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K50" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="L50" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="51">
@@ -2554,6 +2707,9 @@
       <c r="K51" t="n">
         <v>0</v>
       </c>
+      <c r="L51" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -2590,11 +2746,14 @@
         <v>0</v>
       </c>
       <c r="J52" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K52" t="n">
         <v>2</v>
       </c>
+      <c r="L52" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -2631,10 +2790,13 @@
         <v>1</v>
       </c>
       <c r="J53" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K53" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="L53" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="54">
@@ -2677,6 +2839,9 @@
       <c r="K54" t="n">
         <v>0</v>
       </c>
+      <c r="L54" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -2713,10 +2878,13 @@
         <v>1</v>
       </c>
       <c r="J55" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K55" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="L55" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="56">
@@ -2759,6 +2927,9 @@
       <c r="K56" t="n">
         <v>0</v>
       </c>
+      <c r="L56" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -2795,10 +2966,13 @@
         <v>1</v>
       </c>
       <c r="J57" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K57" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="L57" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="58">
@@ -2836,10 +3010,13 @@
         <v>1</v>
       </c>
       <c r="J58" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K58" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="L58" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="59">
@@ -2877,11 +3054,14 @@
         <v>1</v>
       </c>
       <c r="J59" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K59" t="n">
         <v>2</v>
       </c>
+      <c r="L59" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -2918,10 +3098,13 @@
         <v>1</v>
       </c>
       <c r="J60" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K60" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="L60" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="61">
@@ -2959,9 +3142,12 @@
         <v>0</v>
       </c>
       <c r="J61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K61" t="n">
+        <v>1</v>
+      </c>
+      <c r="L61" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3005,6 +3191,9 @@
       <c r="K62" t="n">
         <v>0</v>
       </c>
+      <c r="L62" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -3041,10 +3230,13 @@
         <v>0</v>
       </c>
       <c r="J63" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K63" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="L63" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="64">
@@ -3082,10 +3274,13 @@
         <v>1</v>
       </c>
       <c r="J64" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K64" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="L64" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="65">
@@ -3128,6 +3323,9 @@
       <c r="K65" t="n">
         <v>0</v>
       </c>
+      <c r="L65" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -3169,6 +3367,9 @@
       <c r="K66" t="n">
         <v>0</v>
       </c>
+      <c r="L66" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -3205,9 +3406,12 @@
         <v>1</v>
       </c>
       <c r="J67" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K67" t="n">
+        <v>1</v>
+      </c>
+      <c r="L67" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3251,6 +3455,9 @@
       <c r="K68" t="n">
         <v>0</v>
       </c>
+      <c r="L68" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -3292,6 +3499,9 @@
       <c r="K69" t="n">
         <v>0</v>
       </c>
+      <c r="L69" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -3328,10 +3538,13 @@
         <v>1</v>
       </c>
       <c r="J70" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K70" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="L70" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="71">
@@ -3369,9 +3582,12 @@
         <v>1</v>
       </c>
       <c r="J71" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K71" t="n">
+        <v>1</v>
+      </c>
+      <c r="L71" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3415,6 +3631,9 @@
       <c r="K72" t="n">
         <v>0</v>
       </c>
+      <c r="L72" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -3451,10 +3670,13 @@
         <v>0</v>
       </c>
       <c r="J73" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K73" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="L73" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="74">
@@ -3492,10 +3714,13 @@
         <v>1</v>
       </c>
       <c r="J74" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="K74" t="n">
-        <v>3</v>
+        <v>16</v>
+      </c>
+      <c r="L74" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="75">
@@ -3538,6 +3763,9 @@
       <c r="K75" t="n">
         <v>0</v>
       </c>
+      <c r="L75" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -3574,11 +3802,14 @@
         <v>1</v>
       </c>
       <c r="J76" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K76" t="n">
         <v>2</v>
       </c>
+      <c r="L76" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -3620,6 +3851,9 @@
       <c r="K77" t="n">
         <v>0</v>
       </c>
+      <c r="L77" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -3661,6 +3895,9 @@
       <c r="K78" t="n">
         <v>0</v>
       </c>
+      <c r="L78" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -3697,9 +3934,12 @@
         <v>1</v>
       </c>
       <c r="J79" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K79" t="n">
+        <v>1</v>
+      </c>
+      <c r="L79" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3738,10 +3978,13 @@
         <v>1</v>
       </c>
       <c r="J80" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K80" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="L80" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="81">
@@ -3779,10 +4022,13 @@
         <v>1</v>
       </c>
       <c r="J81" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K81" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="L81" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="82">
@@ -3820,10 +4066,13 @@
         <v>1</v>
       </c>
       <c r="J82" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K82" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="L82" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="83">
@@ -3861,10 +4110,13 @@
         <v>0</v>
       </c>
       <c r="J83" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K83" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="L83" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="84">
@@ -3902,9 +4154,12 @@
         <v>0</v>
       </c>
       <c r="J84" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K84" t="n">
+        <v>1</v>
+      </c>
+      <c r="L84" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3948,6 +4203,9 @@
       <c r="K85" t="n">
         <v>0</v>
       </c>
+      <c r="L85" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -3984,11 +4242,14 @@
         <v>1</v>
       </c>
       <c r="J86" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K86" t="n">
         <v>2</v>
       </c>
+      <c r="L86" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -4030,6 +4291,9 @@
       <c r="K87" t="n">
         <v>0</v>
       </c>
+      <c r="L87" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -4066,11 +4330,14 @@
         <v>1</v>
       </c>
       <c r="J88" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K88" t="n">
         <v>2</v>
       </c>
+      <c r="L88" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -4112,6 +4379,9 @@
       <c r="K89" t="n">
         <v>0</v>
       </c>
+      <c r="L89" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -4148,9 +4418,12 @@
         <v>1</v>
       </c>
       <c r="J90" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K90" t="n">
+        <v>1</v>
+      </c>
+      <c r="L90" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4194,6 +4467,9 @@
       <c r="K91" t="n">
         <v>0</v>
       </c>
+      <c r="L91" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -4235,6 +4511,9 @@
       <c r="K92" t="n">
         <v>0</v>
       </c>
+      <c r="L92" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -4271,9 +4550,12 @@
         <v>1</v>
       </c>
       <c r="J93" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K93" t="n">
+        <v>1</v>
+      </c>
+      <c r="L93" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4312,11 +4594,14 @@
         <v>1</v>
       </c>
       <c r="J94" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K94" t="n">
         <v>2</v>
       </c>
+      <c r="L94" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -4353,9 +4638,12 @@
         <v>1</v>
       </c>
       <c r="J95" t="n">
+        <v>0</v>
+      </c>
+      <c r="K95" t="n">
         <v>32</v>
       </c>
-      <c r="K95" t="n">
+      <c r="L95" t="n">
         <v>3</v>
       </c>
     </row>
@@ -4399,6 +4687,9 @@
       <c r="K96" t="n">
         <v>0</v>
       </c>
+      <c r="L96" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -4440,6 +4731,9 @@
       <c r="K97" t="n">
         <v>0</v>
       </c>
+      <c r="L97" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -4476,10 +4770,13 @@
         <v>0</v>
       </c>
       <c r="J98" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K98" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="L98" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="99">
@@ -4522,6 +4819,9 @@
       <c r="K99" t="n">
         <v>0</v>
       </c>
+      <c r="L99" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -4558,9 +4858,12 @@
         <v>0</v>
       </c>
       <c r="J100" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K100" t="n">
+        <v>1</v>
+      </c>
+      <c r="L100" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4599,10 +4902,13 @@
         <v>1</v>
       </c>
       <c r="J101" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K101" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="L101" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="102">
@@ -4645,6 +4951,9 @@
       <c r="K102" t="n">
         <v>0</v>
       </c>
+      <c r="L102" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -4681,10 +4990,13 @@
         <v>1</v>
       </c>
       <c r="J103" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K103" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="L103" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="104">
@@ -4722,9 +5034,12 @@
         <v>0</v>
       </c>
       <c r="J104" t="n">
+        <v>0</v>
+      </c>
+      <c r="K104" t="n">
         <v>12</v>
       </c>
-      <c r="K104" t="n">
+      <c r="L104" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4763,10 +5078,13 @@
         <v>1</v>
       </c>
       <c r="J105" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K105" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="L105" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="106">
@@ -4804,10 +5122,13 @@
         <v>1</v>
       </c>
       <c r="J106" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K106" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="L106" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="107">
@@ -4850,6 +5171,9 @@
       <c r="K107" t="n">
         <v>0</v>
       </c>
+      <c r="L107" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -4886,10 +5210,13 @@
         <v>1</v>
       </c>
       <c r="J108" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K108" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="L108" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="109">
@@ -4930,6 +5257,9 @@
         <v>0</v>
       </c>
       <c r="K109" t="n">
+        <v>0</v>
+      </c>
+      <c r="L109" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Daily IST report: add CSV/MD/XLSX (#844)
Co-authored-by: codethesept <198977775+codethesept@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/reports/submissions_daily_matrix.xlsx
+++ b/reports/submissions_daily_matrix.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L109"/>
+  <dimension ref="A1:M109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,8 +445,9 @@
     <col width="12" customWidth="1" min="8" max="8"/>
     <col width="12" customWidth="1" min="9" max="9"/>
     <col width="12" customWidth="1" min="10" max="10"/>
-    <col width="13" customWidth="1" min="11" max="11"/>
+    <col width="12" customWidth="1" min="11" max="11"/>
     <col width="13" customWidth="1" min="12" max="12"/>
+    <col width="13" customWidth="1" min="13" max="13"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -500,12 +501,17 @@
           <t>2026-02-24</t>
         </is>
       </c>
-      <c r="K1" s="2" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>2026-02-25</t>
+        </is>
+      </c>
+      <c r="L1" s="2" t="inlineStr">
         <is>
           <t>total_files</t>
         </is>
       </c>
-      <c r="L1" s="2" t="inlineStr">
+      <c r="M1" s="2" t="inlineStr">
         <is>
           <t>unique_days</t>
         </is>
@@ -549,10 +555,13 @@
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L2" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="M2" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="3">
@@ -593,10 +602,13 @@
         <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L3" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="M3" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="4">
@@ -637,10 +649,13 @@
         <v>1</v>
       </c>
       <c r="K4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L4" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="M4" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="5">
@@ -681,10 +696,13 @@
         <v>1</v>
       </c>
       <c r="K5" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L5" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="M5" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="6">
@@ -725,10 +743,13 @@
         <v>1</v>
       </c>
       <c r="K6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L6" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="M6" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="7">
@@ -769,10 +790,13 @@
         <v>1</v>
       </c>
       <c r="K7" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L7" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="M7" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="8">
@@ -813,10 +837,13 @@
         <v>1</v>
       </c>
       <c r="K8" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L8" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="M8" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="9">
@@ -857,10 +884,13 @@
         <v>1</v>
       </c>
       <c r="K9" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L9" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="M9" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="10">
@@ -901,10 +931,13 @@
         <v>1</v>
       </c>
       <c r="K10" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L10" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="M10" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="11">
@@ -945,10 +978,13 @@
         <v>1</v>
       </c>
       <c r="K11" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L11" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="M11" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="12">
@@ -989,10 +1025,13 @@
         <v>1</v>
       </c>
       <c r="K12" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L12" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="M12" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="13">
@@ -1033,10 +1072,13 @@
         <v>1</v>
       </c>
       <c r="K13" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L13" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="M13" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="14">
@@ -1077,10 +1119,13 @@
         <v>1</v>
       </c>
       <c r="K14" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L14" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="M14" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="15">
@@ -1121,10 +1166,13 @@
         <v>0</v>
       </c>
       <c r="K15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L15" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="M15" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="16">
@@ -1165,10 +1213,13 @@
         <v>1</v>
       </c>
       <c r="K16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L16" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="M16" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="17">
@@ -1209,10 +1260,13 @@
         <v>1</v>
       </c>
       <c r="K17" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L17" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="M17" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="18">
@@ -1253,10 +1307,13 @@
         <v>1</v>
       </c>
       <c r="K18" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L18" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="M18" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="19">
@@ -1297,11 +1354,14 @@
         <v>1</v>
       </c>
       <c r="K19" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L19" t="n">
         <v>3</v>
       </c>
+      <c r="M19" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1341,10 +1401,13 @@
         <v>1</v>
       </c>
       <c r="K20" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L20" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="M20" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="21">
@@ -1390,6 +1453,9 @@
       <c r="L21" t="n">
         <v>0</v>
       </c>
+      <c r="M21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1434,6 +1500,9 @@
       <c r="L22" t="n">
         <v>0</v>
       </c>
+      <c r="M22" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1478,6 +1547,9 @@
       <c r="L23" t="n">
         <v>0</v>
       </c>
+      <c r="M23" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1517,10 +1589,13 @@
         <v>1</v>
       </c>
       <c r="K24" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L24" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="M24" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="25">
@@ -1561,10 +1636,13 @@
         <v>0</v>
       </c>
       <c r="K25" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L25" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="M25" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="26">
@@ -1608,7 +1686,10 @@
         <v>1</v>
       </c>
       <c r="L26" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="M26" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="27">
@@ -1649,10 +1730,13 @@
         <v>1</v>
       </c>
       <c r="K27" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L27" t="n">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="M27" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="28">
@@ -1698,6 +1782,9 @@
       <c r="L28" t="n">
         <v>0</v>
       </c>
+      <c r="M28" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1742,6 +1829,9 @@
       <c r="L29" t="n">
         <v>0</v>
       </c>
+      <c r="M29" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1786,6 +1876,9 @@
       <c r="L30" t="n">
         <v>0</v>
       </c>
+      <c r="M30" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1825,10 +1918,13 @@
         <v>1</v>
       </c>
       <c r="K31" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L31" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="M31" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="32">
@@ -1869,10 +1965,13 @@
         <v>1</v>
       </c>
       <c r="K32" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L32" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="M32" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="33">
@@ -1913,10 +2012,13 @@
         <v>1</v>
       </c>
       <c r="K33" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L33" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="M33" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="34">
@@ -1957,10 +2059,13 @@
         <v>1</v>
       </c>
       <c r="K34" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L34" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="M34" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="35">
@@ -2001,11 +2106,14 @@
         <v>1</v>
       </c>
       <c r="K35" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L35" t="n">
         <v>4</v>
       </c>
+      <c r="M35" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -2045,10 +2153,13 @@
         <v>1</v>
       </c>
       <c r="K36" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L36" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="M36" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="37">
@@ -2089,11 +2200,14 @@
         <v>1</v>
       </c>
       <c r="K37" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L37" t="n">
         <v>2</v>
       </c>
+      <c r="M37" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -2138,6 +2252,9 @@
       <c r="L38" t="n">
         <v>0</v>
       </c>
+      <c r="M38" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -2182,6 +2299,9 @@
       <c r="L39" t="n">
         <v>0</v>
       </c>
+      <c r="M39" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -2221,10 +2341,13 @@
         <v>1</v>
       </c>
       <c r="K40" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L40" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="M40" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="41">
@@ -2265,10 +2388,13 @@
         <v>1</v>
       </c>
       <c r="K41" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L41" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="M41" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="42">
@@ -2309,10 +2435,13 @@
         <v>1</v>
       </c>
       <c r="K42" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L42" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="M42" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="43">
@@ -2353,9 +2482,12 @@
         <v>0</v>
       </c>
       <c r="K43" t="n">
+        <v>0</v>
+      </c>
+      <c r="L43" t="n">
         <v>21</v>
       </c>
-      <c r="L43" t="n">
+      <c r="M43" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2397,10 +2529,13 @@
         <v>42</v>
       </c>
       <c r="K44" t="n">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="L44" t="n">
-        <v>1</v>
+        <v>43</v>
+      </c>
+      <c r="M44" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="45">
@@ -2441,11 +2576,14 @@
         <v>0</v>
       </c>
       <c r="K45" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L45" t="n">
         <v>2</v>
       </c>
+      <c r="M45" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2485,10 +2623,13 @@
         <v>1</v>
       </c>
       <c r="K46" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L46" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="M46" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="47">
@@ -2529,10 +2670,13 @@
         <v>1</v>
       </c>
       <c r="K47" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L47" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="M47" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="48">
@@ -2578,6 +2722,9 @@
       <c r="L48" t="n">
         <v>0</v>
       </c>
+      <c r="M48" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2617,10 +2764,13 @@
         <v>1</v>
       </c>
       <c r="K49" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L49" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="M49" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="50">
@@ -2661,10 +2811,13 @@
         <v>1</v>
       </c>
       <c r="K50" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L50" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="M50" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="51">
@@ -2710,6 +2863,9 @@
       <c r="L51" t="n">
         <v>0</v>
       </c>
+      <c r="M51" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -2749,11 +2905,14 @@
         <v>0</v>
       </c>
       <c r="K52" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L52" t="n">
         <v>2</v>
       </c>
+      <c r="M52" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -2793,10 +2952,13 @@
         <v>1</v>
       </c>
       <c r="K53" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L53" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="M53" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="54">
@@ -2842,6 +3004,9 @@
       <c r="L54" t="n">
         <v>0</v>
       </c>
+      <c r="M54" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -2881,10 +3046,13 @@
         <v>1</v>
       </c>
       <c r="K55" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L55" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="M55" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="56">
@@ -2930,6 +3098,9 @@
       <c r="L56" t="n">
         <v>0</v>
       </c>
+      <c r="M56" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -2969,10 +3140,13 @@
         <v>1</v>
       </c>
       <c r="K57" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L57" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="M57" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="58">
@@ -3013,10 +3187,13 @@
         <v>1</v>
       </c>
       <c r="K58" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L58" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="M58" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="59">
@@ -3057,10 +3234,13 @@
         <v>0</v>
       </c>
       <c r="K59" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L59" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="M59" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="60">
@@ -3101,10 +3281,13 @@
         <v>1</v>
       </c>
       <c r="K60" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L60" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="M60" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="61">
@@ -3145,9 +3328,12 @@
         <v>0</v>
       </c>
       <c r="K61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L61" t="n">
+        <v>1</v>
+      </c>
+      <c r="M61" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3194,6 +3380,9 @@
       <c r="L62" t="n">
         <v>0</v>
       </c>
+      <c r="M62" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -3236,7 +3425,10 @@
         <v>1</v>
       </c>
       <c r="L63" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="M63" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="64">
@@ -3277,10 +3469,13 @@
         <v>1</v>
       </c>
       <c r="K64" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L64" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="M64" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="65">
@@ -3326,6 +3521,9 @@
       <c r="L65" t="n">
         <v>0</v>
       </c>
+      <c r="M65" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -3370,6 +3568,9 @@
       <c r="L66" t="n">
         <v>0</v>
       </c>
+      <c r="M66" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -3412,7 +3613,10 @@
         <v>1</v>
       </c>
       <c r="L67" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="M67" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="68">
@@ -3458,6 +3662,9 @@
       <c r="L68" t="n">
         <v>0</v>
       </c>
+      <c r="M68" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -3502,6 +3709,9 @@
       <c r="L69" t="n">
         <v>0</v>
       </c>
+      <c r="M69" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -3541,10 +3751,13 @@
         <v>1</v>
       </c>
       <c r="K70" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L70" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="M70" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="71">
@@ -3585,9 +3798,12 @@
         <v>0</v>
       </c>
       <c r="K71" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L71" t="n">
+        <v>1</v>
+      </c>
+      <c r="M71" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3634,6 +3850,9 @@
       <c r="L72" t="n">
         <v>0</v>
       </c>
+      <c r="M72" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -3676,7 +3895,10 @@
         <v>1</v>
       </c>
       <c r="L73" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="M73" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="74">
@@ -3717,9 +3939,12 @@
         <v>1</v>
       </c>
       <c r="K74" t="n">
+        <v>0</v>
+      </c>
+      <c r="L74" t="n">
         <v>16</v>
       </c>
-      <c r="L74" t="n">
+      <c r="M74" t="n">
         <v>4</v>
       </c>
     </row>
@@ -3766,6 +3991,9 @@
       <c r="L75" t="n">
         <v>0</v>
       </c>
+      <c r="M75" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -3805,10 +4033,13 @@
         <v>0</v>
       </c>
       <c r="K76" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L76" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="M76" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="77">
@@ -3854,6 +4085,9 @@
       <c r="L77" t="n">
         <v>0</v>
       </c>
+      <c r="M77" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -3898,6 +4132,9 @@
       <c r="L78" t="n">
         <v>0</v>
       </c>
+      <c r="M78" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -3940,7 +4177,10 @@
         <v>1</v>
       </c>
       <c r="L79" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="M79" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="80">
@@ -3981,10 +4221,13 @@
         <v>1</v>
       </c>
       <c r="K80" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L80" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="M80" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="81">
@@ -4025,10 +4268,13 @@
         <v>1</v>
       </c>
       <c r="K81" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L81" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="M81" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="82">
@@ -4069,10 +4315,13 @@
         <v>1</v>
       </c>
       <c r="K82" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L82" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="M82" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="83">
@@ -4116,7 +4365,10 @@
         <v>1</v>
       </c>
       <c r="L83" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="M83" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="84">
@@ -4157,9 +4409,12 @@
         <v>0</v>
       </c>
       <c r="K84" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L84" t="n">
+        <v>1</v>
+      </c>
+      <c r="M84" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4206,6 +4461,9 @@
       <c r="L85" t="n">
         <v>0</v>
       </c>
+      <c r="M85" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -4245,11 +4503,14 @@
         <v>0</v>
       </c>
       <c r="K86" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L86" t="n">
         <v>2</v>
       </c>
+      <c r="M86" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -4294,6 +4555,9 @@
       <c r="L87" t="n">
         <v>0</v>
       </c>
+      <c r="M87" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -4333,11 +4597,14 @@
         <v>0</v>
       </c>
       <c r="K88" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L88" t="n">
         <v>2</v>
       </c>
+      <c r="M88" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -4382,6 +4649,9 @@
       <c r="L89" t="n">
         <v>0</v>
       </c>
+      <c r="M89" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -4421,9 +4691,12 @@
         <v>0</v>
       </c>
       <c r="K90" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L90" t="n">
+        <v>1</v>
+      </c>
+      <c r="M90" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4470,6 +4743,9 @@
       <c r="L91" t="n">
         <v>0</v>
       </c>
+      <c r="M91" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -4514,6 +4790,9 @@
       <c r="L92" t="n">
         <v>0</v>
       </c>
+      <c r="M92" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -4556,7 +4835,10 @@
         <v>1</v>
       </c>
       <c r="L93" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="M93" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="94">
@@ -4597,10 +4879,13 @@
         <v>0</v>
       </c>
       <c r="K94" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L94" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="M94" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="95">
@@ -4641,9 +4926,12 @@
         <v>0</v>
       </c>
       <c r="K95" t="n">
+        <v>0</v>
+      </c>
+      <c r="L95" t="n">
         <v>32</v>
       </c>
-      <c r="L95" t="n">
+      <c r="M95" t="n">
         <v>3</v>
       </c>
     </row>
@@ -4685,10 +4973,13 @@
         <v>0</v>
       </c>
       <c r="K96" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L96" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="M96" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="97">
@@ -4734,6 +5025,9 @@
       <c r="L97" t="n">
         <v>0</v>
       </c>
+      <c r="M97" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -4773,9 +5067,12 @@
         <v>1</v>
       </c>
       <c r="K98" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L98" t="n">
+        <v>1</v>
+      </c>
+      <c r="M98" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4822,6 +5119,9 @@
       <c r="L99" t="n">
         <v>0</v>
       </c>
+      <c r="M99" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -4864,7 +5164,10 @@
         <v>1</v>
       </c>
       <c r="L100" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="M100" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="101">
@@ -4905,10 +5208,13 @@
         <v>1</v>
       </c>
       <c r="K101" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L101" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="M101" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="102">
@@ -4954,6 +5260,9 @@
       <c r="L102" t="n">
         <v>0</v>
       </c>
+      <c r="M102" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -4993,10 +5302,13 @@
         <v>1</v>
       </c>
       <c r="K103" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L103" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="M103" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="104">
@@ -5037,9 +5349,12 @@
         <v>0</v>
       </c>
       <c r="K104" t="n">
+        <v>0</v>
+      </c>
+      <c r="L104" t="n">
         <v>12</v>
       </c>
-      <c r="L104" t="n">
+      <c r="M104" t="n">
         <v>1</v>
       </c>
     </row>
@@ -5081,10 +5396,13 @@
         <v>1</v>
       </c>
       <c r="K105" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L105" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="M105" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="106">
@@ -5125,10 +5443,13 @@
         <v>1</v>
       </c>
       <c r="K106" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L106" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="M106" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="107">
@@ -5174,6 +5495,9 @@
       <c r="L107" t="n">
         <v>0</v>
       </c>
+      <c r="M107" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -5213,10 +5537,13 @@
         <v>1</v>
       </c>
       <c r="K108" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L108" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="M108" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="109">
@@ -5260,6 +5587,9 @@
         <v>0</v>
       </c>
       <c r="L109" t="n">
+        <v>0</v>
+      </c>
+      <c r="M109" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Daily IST report: add CSV/MD/XLSX (#950)
Co-authored-by: codethesept <198977775+codethesept@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/reports/submissions_daily_matrix.xlsx
+++ b/reports/submissions_daily_matrix.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M109"/>
+  <dimension ref="A1:N109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,8 +446,9 @@
     <col width="12" customWidth="1" min="9" max="9"/>
     <col width="12" customWidth="1" min="10" max="10"/>
     <col width="12" customWidth="1" min="11" max="11"/>
-    <col width="13" customWidth="1" min="12" max="12"/>
+    <col width="12" customWidth="1" min="12" max="12"/>
     <col width="13" customWidth="1" min="13" max="13"/>
+    <col width="13" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -506,12 +507,17 @@
           <t>2026-02-25</t>
         </is>
       </c>
-      <c r="L1" s="2" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>2026-02-26</t>
+        </is>
+      </c>
+      <c r="M1" s="2" t="inlineStr">
         <is>
           <t>total_files</t>
         </is>
       </c>
-      <c r="M1" s="2" t="inlineStr">
+      <c r="N1" s="2" t="inlineStr">
         <is>
           <t>unique_days</t>
         </is>
@@ -558,10 +564,13 @@
         <v>1</v>
       </c>
       <c r="L2" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M2" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="N2" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="3">
@@ -605,10 +614,13 @@
         <v>1</v>
       </c>
       <c r="L3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M3" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="N3" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="4">
@@ -652,10 +664,13 @@
         <v>1</v>
       </c>
       <c r="L4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M4" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="N4" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="5">
@@ -699,10 +714,13 @@
         <v>1</v>
       </c>
       <c r="L5" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M5" t="n">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="N5" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="6">
@@ -746,10 +764,13 @@
         <v>1</v>
       </c>
       <c r="L6" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M6" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="N6" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="7">
@@ -793,10 +814,13 @@
         <v>1</v>
       </c>
       <c r="L7" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M7" t="n">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="N7" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="8">
@@ -840,10 +864,13 @@
         <v>1</v>
       </c>
       <c r="L8" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M8" t="n">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="N8" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="9">
@@ -887,10 +914,13 @@
         <v>1</v>
       </c>
       <c r="L9" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M9" t="n">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="N9" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="10">
@@ -934,10 +964,13 @@
         <v>1</v>
       </c>
       <c r="L10" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M10" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="N10" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="11">
@@ -981,10 +1014,13 @@
         <v>1</v>
       </c>
       <c r="L11" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M11" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="N11" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="12">
@@ -1028,10 +1064,13 @@
         <v>1</v>
       </c>
       <c r="L12" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M12" t="n">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="N12" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="13">
@@ -1075,10 +1114,13 @@
         <v>1</v>
       </c>
       <c r="L13" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M13" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="N13" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="14">
@@ -1122,10 +1164,13 @@
         <v>1</v>
       </c>
       <c r="L14" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M14" t="n">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="N14" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="15">
@@ -1169,10 +1214,13 @@
         <v>1</v>
       </c>
       <c r="L15" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M15" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="N15" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="16">
@@ -1216,10 +1264,13 @@
         <v>1</v>
       </c>
       <c r="L16" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M16" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="N16" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="17">
@@ -1263,10 +1314,13 @@
         <v>1</v>
       </c>
       <c r="L17" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M17" t="n">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="N17" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="18">
@@ -1310,10 +1364,13 @@
         <v>1</v>
       </c>
       <c r="L18" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M18" t="n">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="N18" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="19">
@@ -1357,10 +1414,13 @@
         <v>0</v>
       </c>
       <c r="L19" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M19" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="N19" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="20">
@@ -1404,10 +1464,13 @@
         <v>1</v>
       </c>
       <c r="L20" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M20" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="N20" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="21">
@@ -1456,6 +1519,9 @@
       <c r="M21" t="n">
         <v>0</v>
       </c>
+      <c r="N21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1503,6 +1569,9 @@
       <c r="M22" t="n">
         <v>0</v>
       </c>
+      <c r="N22" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1545,10 +1614,13 @@
         <v>0</v>
       </c>
       <c r="L23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M23" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="N23" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="24">
@@ -1592,10 +1664,13 @@
         <v>1</v>
       </c>
       <c r="L24" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M24" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="N24" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="25">
@@ -1639,11 +1714,14 @@
         <v>1</v>
       </c>
       <c r="L25" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M25" t="n">
         <v>4</v>
       </c>
+      <c r="N25" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1686,10 +1764,13 @@
         <v>1</v>
       </c>
       <c r="L26" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M26" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="N26" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="27">
@@ -1733,10 +1814,13 @@
         <v>1</v>
       </c>
       <c r="L27" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="M27" t="n">
-        <v>4</v>
+        <v>7</v>
+      </c>
+      <c r="N27" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="28">
@@ -1785,6 +1869,9 @@
       <c r="M28" t="n">
         <v>0</v>
       </c>
+      <c r="N28" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1832,6 +1919,9 @@
       <c r="M29" t="n">
         <v>0</v>
       </c>
+      <c r="N29" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1879,6 +1969,9 @@
       <c r="M30" t="n">
         <v>0</v>
       </c>
+      <c r="N30" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1921,10 +2014,13 @@
         <v>1</v>
       </c>
       <c r="L31" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M31" t="n">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="N31" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="32">
@@ -1968,10 +2064,13 @@
         <v>1</v>
       </c>
       <c r="L32" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M32" t="n">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="N32" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="33">
@@ -2015,10 +2114,13 @@
         <v>1</v>
       </c>
       <c r="L33" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M33" t="n">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="N33" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="34">
@@ -2062,10 +2164,13 @@
         <v>1</v>
       </c>
       <c r="L34" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M34" t="n">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="N34" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="35">
@@ -2109,10 +2214,13 @@
         <v>0</v>
       </c>
       <c r="L35" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M35" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="N35" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="36">
@@ -2156,10 +2264,13 @@
         <v>1</v>
       </c>
       <c r="L36" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M36" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="N36" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="37">
@@ -2203,10 +2314,13 @@
         <v>0</v>
       </c>
       <c r="L37" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M37" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="N37" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="38">
@@ -2255,6 +2369,9 @@
       <c r="M38" t="n">
         <v>0</v>
       </c>
+      <c r="N38" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -2302,6 +2419,9 @@
       <c r="M39" t="n">
         <v>0</v>
       </c>
+      <c r="N39" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -2344,10 +2464,13 @@
         <v>1</v>
       </c>
       <c r="L40" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M40" t="n">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="N40" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="41">
@@ -2391,10 +2514,13 @@
         <v>1</v>
       </c>
       <c r="L41" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M41" t="n">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="N41" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="42">
@@ -2438,10 +2564,13 @@
         <v>1</v>
       </c>
       <c r="L42" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M42" t="n">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="N42" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="43">
@@ -2485,9 +2614,12 @@
         <v>0</v>
       </c>
       <c r="L43" t="n">
+        <v>0</v>
+      </c>
+      <c r="M43" t="n">
         <v>21</v>
       </c>
-      <c r="M43" t="n">
+      <c r="N43" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2532,10 +2664,13 @@
         <v>1</v>
       </c>
       <c r="L44" t="n">
-        <v>43</v>
+        <v>1</v>
       </c>
       <c r="M44" t="n">
-        <v>2</v>
+        <v>44</v>
+      </c>
+      <c r="N44" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="45">
@@ -2579,10 +2714,13 @@
         <v>0</v>
       </c>
       <c r="L45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M45" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="N45" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="46">
@@ -2626,10 +2764,13 @@
         <v>1</v>
       </c>
       <c r="L46" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M46" t="n">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="N46" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="47">
@@ -2673,10 +2814,13 @@
         <v>1</v>
       </c>
       <c r="L47" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M47" t="n">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="N47" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="48">
@@ -2725,6 +2869,9 @@
       <c r="M48" t="n">
         <v>0</v>
       </c>
+      <c r="N48" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2767,10 +2914,13 @@
         <v>1</v>
       </c>
       <c r="L49" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M49" t="n">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="N49" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="50">
@@ -2814,10 +2964,13 @@
         <v>1</v>
       </c>
       <c r="L50" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M50" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="N50" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="51">
@@ -2861,10 +3014,13 @@
         <v>0</v>
       </c>
       <c r="L51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M51" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="N51" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="52">
@@ -2908,11 +3064,14 @@
         <v>0</v>
       </c>
       <c r="L52" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M52" t="n">
         <v>2</v>
       </c>
+      <c r="N52" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -2955,10 +3114,13 @@
         <v>1</v>
       </c>
       <c r="L53" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M53" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="N53" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="54">
@@ -3007,6 +3169,9 @@
       <c r="M54" t="n">
         <v>0</v>
       </c>
+      <c r="N54" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -3049,10 +3214,13 @@
         <v>1</v>
       </c>
       <c r="L55" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M55" t="n">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="N55" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="56">
@@ -3101,6 +3269,9 @@
       <c r="M56" t="n">
         <v>0</v>
       </c>
+      <c r="N56" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -3143,10 +3314,13 @@
         <v>1</v>
       </c>
       <c r="L57" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M57" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="N57" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="58">
@@ -3190,10 +3364,13 @@
         <v>1</v>
       </c>
       <c r="L58" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M58" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="N58" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="59">
@@ -3237,11 +3414,14 @@
         <v>1</v>
       </c>
       <c r="L59" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M59" t="n">
         <v>3</v>
       </c>
+      <c r="N59" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -3284,10 +3464,13 @@
         <v>1</v>
       </c>
       <c r="L60" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M60" t="n">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="N60" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="61">
@@ -3331,9 +3514,12 @@
         <v>0</v>
       </c>
       <c r="L61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M61" t="n">
+        <v>1</v>
+      </c>
+      <c r="N61" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3383,6 +3569,9 @@
       <c r="M62" t="n">
         <v>0</v>
       </c>
+      <c r="N62" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -3425,10 +3614,13 @@
         <v>1</v>
       </c>
       <c r="L63" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M63" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="N63" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="64">
@@ -3472,10 +3664,13 @@
         <v>1</v>
       </c>
       <c r="L64" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M64" t="n">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="N64" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="65">
@@ -3524,6 +3719,9 @@
       <c r="M65" t="n">
         <v>0</v>
       </c>
+      <c r="N65" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -3571,6 +3769,9 @@
       <c r="M66" t="n">
         <v>0</v>
       </c>
+      <c r="N66" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -3613,11 +3814,14 @@
         <v>1</v>
       </c>
       <c r="L67" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M67" t="n">
         <v>2</v>
       </c>
+      <c r="N67" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -3665,6 +3869,9 @@
       <c r="M68" t="n">
         <v>0</v>
       </c>
+      <c r="N68" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -3712,6 +3919,9 @@
       <c r="M69" t="n">
         <v>0</v>
       </c>
+      <c r="N69" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -3754,10 +3964,13 @@
         <v>1</v>
       </c>
       <c r="L70" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M70" t="n">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="N70" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="71">
@@ -3801,9 +4014,12 @@
         <v>0</v>
       </c>
       <c r="L71" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M71" t="n">
+        <v>1</v>
+      </c>
+      <c r="N71" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3853,6 +4069,9 @@
       <c r="M72" t="n">
         <v>0</v>
       </c>
+      <c r="N72" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -3895,10 +4114,13 @@
         <v>1</v>
       </c>
       <c r="L73" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M73" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="N73" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="74">
@@ -3942,10 +4164,13 @@
         <v>0</v>
       </c>
       <c r="L74" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="M74" t="n">
-        <v>4</v>
+        <v>17</v>
+      </c>
+      <c r="N74" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="75">
@@ -3989,10 +4214,13 @@
         <v>0</v>
       </c>
       <c r="L75" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M75" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="N75" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="76">
@@ -4036,10 +4264,13 @@
         <v>1</v>
       </c>
       <c r="L76" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M76" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="N76" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="77">
@@ -4088,6 +4319,9 @@
       <c r="M77" t="n">
         <v>0</v>
       </c>
+      <c r="N77" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -4135,6 +4369,9 @@
       <c r="M78" t="n">
         <v>0</v>
       </c>
+      <c r="N78" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -4177,10 +4414,13 @@
         <v>1</v>
       </c>
       <c r="L79" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M79" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="N79" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="80">
@@ -4224,10 +4464,13 @@
         <v>1</v>
       </c>
       <c r="L80" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M80" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="N80" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="81">
@@ -4271,11 +4514,14 @@
         <v>1</v>
       </c>
       <c r="L81" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M81" t="n">
         <v>4</v>
       </c>
+      <c r="N81" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -4318,10 +4564,13 @@
         <v>1</v>
       </c>
       <c r="L82" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M82" t="n">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="N82" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="83">
@@ -4365,10 +4614,13 @@
         <v>1</v>
       </c>
       <c r="L83" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M83" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="N83" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="84">
@@ -4412,9 +4664,12 @@
         <v>0</v>
       </c>
       <c r="L84" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M84" t="n">
+        <v>1</v>
+      </c>
+      <c r="N84" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4464,6 +4719,9 @@
       <c r="M85" t="n">
         <v>0</v>
       </c>
+      <c r="N85" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -4506,10 +4764,13 @@
         <v>0</v>
       </c>
       <c r="L86" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M86" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="N86" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="87">
@@ -4558,6 +4819,9 @@
       <c r="M87" t="n">
         <v>0</v>
       </c>
+      <c r="N87" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -4600,11 +4864,14 @@
         <v>0</v>
       </c>
       <c r="L88" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M88" t="n">
         <v>2</v>
       </c>
+      <c r="N88" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -4652,6 +4919,9 @@
       <c r="M89" t="n">
         <v>0</v>
       </c>
+      <c r="N89" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -4697,7 +4967,10 @@
         <v>1</v>
       </c>
       <c r="M90" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="N90" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="91">
@@ -4746,6 +5019,9 @@
       <c r="M91" t="n">
         <v>0</v>
       </c>
+      <c r="N91" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -4793,6 +5069,9 @@
       <c r="M92" t="n">
         <v>0</v>
       </c>
+      <c r="N92" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -4835,10 +5114,13 @@
         <v>1</v>
       </c>
       <c r="L93" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M93" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="N93" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="94">
@@ -4882,10 +5164,13 @@
         <v>1</v>
       </c>
       <c r="L94" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M94" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="N94" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="95">
@@ -4929,10 +5214,13 @@
         <v>0</v>
       </c>
       <c r="L95" t="n">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="M95" t="n">
-        <v>3</v>
+        <v>33</v>
+      </c>
+      <c r="N95" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="96">
@@ -4976,9 +5264,12 @@
         <v>1</v>
       </c>
       <c r="L96" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M96" t="n">
+        <v>1</v>
+      </c>
+      <c r="N96" t="n">
         <v>1</v>
       </c>
     </row>
@@ -5028,6 +5319,9 @@
       <c r="M97" t="n">
         <v>0</v>
       </c>
+      <c r="N97" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -5073,7 +5367,10 @@
         <v>1</v>
       </c>
       <c r="M98" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="N98" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="99">
@@ -5122,6 +5419,9 @@
       <c r="M99" t="n">
         <v>0</v>
       </c>
+      <c r="N99" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -5164,11 +5464,14 @@
         <v>1</v>
       </c>
       <c r="L100" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M100" t="n">
         <v>2</v>
       </c>
+      <c r="N100" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -5211,10 +5514,13 @@
         <v>1</v>
       </c>
       <c r="L101" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M101" t="n">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="N101" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="102">
@@ -5263,6 +5569,9 @@
       <c r="M102" t="n">
         <v>0</v>
       </c>
+      <c r="N102" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -5305,10 +5614,13 @@
         <v>1</v>
       </c>
       <c r="L103" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M103" t="n">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="N103" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="104">
@@ -5352,9 +5664,12 @@
         <v>0</v>
       </c>
       <c r="L104" t="n">
+        <v>0</v>
+      </c>
+      <c r="M104" t="n">
         <v>12</v>
       </c>
-      <c r="M104" t="n">
+      <c r="N104" t="n">
         <v>1</v>
       </c>
     </row>
@@ -5399,10 +5714,13 @@
         <v>1</v>
       </c>
       <c r="L105" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M105" t="n">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="N105" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="106">
@@ -5446,10 +5764,13 @@
         <v>1</v>
       </c>
       <c r="L106" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M106" t="n">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="N106" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="107">
@@ -5498,6 +5819,9 @@
       <c r="M107" t="n">
         <v>0</v>
       </c>
+      <c r="N107" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -5540,10 +5864,13 @@
         <v>1</v>
       </c>
       <c r="L108" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M108" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="N108" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="109">
@@ -5590,6 +5917,9 @@
         <v>0</v>
       </c>
       <c r="M109" t="n">
+        <v>0</v>
+      </c>
+      <c r="N109" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Daily IST report: add CSV/MD/XLSX (#1047)
Co-authored-by: codethesept <198977775+codethesept@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/reports/submissions_daily_matrix.xlsx
+++ b/reports/submissions_daily_matrix.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N109"/>
+  <dimension ref="A1:O109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,8 +447,9 @@
     <col width="12" customWidth="1" min="10" max="10"/>
     <col width="12" customWidth="1" min="11" max="11"/>
     <col width="12" customWidth="1" min="12" max="12"/>
-    <col width="13" customWidth="1" min="13" max="13"/>
+    <col width="12" customWidth="1" min="13" max="13"/>
     <col width="13" customWidth="1" min="14" max="14"/>
+    <col width="13" customWidth="1" min="15" max="15"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -512,12 +513,17 @@
           <t>2026-02-26</t>
         </is>
       </c>
-      <c r="M1" s="2" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>2026-02-27</t>
+        </is>
+      </c>
+      <c r="N1" s="2" t="inlineStr">
         <is>
           <t>total_files</t>
         </is>
       </c>
-      <c r="N1" s="2" t="inlineStr">
+      <c r="O1" s="2" t="inlineStr">
         <is>
           <t>unique_days</t>
         </is>
@@ -567,10 +573,13 @@
         <v>1</v>
       </c>
       <c r="M2" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="N2" t="n">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="O2" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="3">
@@ -617,10 +626,13 @@
         <v>1</v>
       </c>
       <c r="M3" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="N3" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="O3" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="4">
@@ -667,10 +679,13 @@
         <v>1</v>
       </c>
       <c r="M4" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="N4" t="n">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="O4" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="5">
@@ -717,10 +732,13 @@
         <v>1</v>
       </c>
       <c r="M5" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="N5" t="n">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="O5" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="6">
@@ -767,10 +785,13 @@
         <v>1</v>
       </c>
       <c r="M6" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="N6" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="O6" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="7">
@@ -817,10 +838,13 @@
         <v>1</v>
       </c>
       <c r="M7" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="N7" t="n">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="O7" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="8">
@@ -867,10 +891,13 @@
         <v>1</v>
       </c>
       <c r="M8" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="N8" t="n">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="O8" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="9">
@@ -917,10 +944,13 @@
         <v>1</v>
       </c>
       <c r="M9" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="N9" t="n">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="O9" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="10">
@@ -967,10 +997,13 @@
         <v>1</v>
       </c>
       <c r="M10" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="N10" t="n">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="O10" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="11">
@@ -1017,10 +1050,13 @@
         <v>1</v>
       </c>
       <c r="M11" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="N11" t="n">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="O11" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="12">
@@ -1067,10 +1103,13 @@
         <v>1</v>
       </c>
       <c r="M12" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="N12" t="n">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="O12" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="13">
@@ -1117,11 +1156,14 @@
         <v>1</v>
       </c>
       <c r="M13" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N13" t="n">
         <v>5</v>
       </c>
+      <c r="O13" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1167,10 +1209,13 @@
         <v>1</v>
       </c>
       <c r="M14" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="N14" t="n">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="O14" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="15">
@@ -1217,10 +1262,13 @@
         <v>1</v>
       </c>
       <c r="M15" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="N15" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="O15" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="16">
@@ -1267,10 +1315,13 @@
         <v>1</v>
       </c>
       <c r="M16" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="N16" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="O16" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="17">
@@ -1317,10 +1368,13 @@
         <v>1</v>
       </c>
       <c r="M17" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="N17" t="n">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="O17" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="18">
@@ -1367,10 +1421,13 @@
         <v>1</v>
       </c>
       <c r="M18" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="N18" t="n">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="O18" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="19">
@@ -1417,10 +1474,13 @@
         <v>1</v>
       </c>
       <c r="M19" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="N19" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="O19" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="20">
@@ -1467,10 +1527,13 @@
         <v>1</v>
       </c>
       <c r="M20" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="N20" t="n">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="O20" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="21">
@@ -1522,6 +1585,9 @@
       <c r="N21" t="n">
         <v>0</v>
       </c>
+      <c r="O21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1572,6 +1638,9 @@
       <c r="N22" t="n">
         <v>0</v>
       </c>
+      <c r="O22" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1620,7 +1689,10 @@
         <v>1</v>
       </c>
       <c r="N23" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="O23" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="24">
@@ -1667,10 +1739,13 @@
         <v>1</v>
       </c>
       <c r="M24" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="N24" t="n">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="O24" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="25">
@@ -1717,10 +1792,13 @@
         <v>0</v>
       </c>
       <c r="M25" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="N25" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="O25" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="26">
@@ -1767,10 +1845,13 @@
         <v>1</v>
       </c>
       <c r="M26" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N26" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="O26" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="27">
@@ -1817,10 +1898,13 @@
         <v>1</v>
       </c>
       <c r="M27" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="N27" t="n">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="O27" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="28">
@@ -1872,6 +1956,9 @@
       <c r="N28" t="n">
         <v>0</v>
       </c>
+      <c r="O28" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1922,6 +2009,9 @@
       <c r="N29" t="n">
         <v>0</v>
       </c>
+      <c r="O29" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1972,6 +2062,9 @@
       <c r="N30" t="n">
         <v>0</v>
       </c>
+      <c r="O30" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -2017,10 +2110,13 @@
         <v>1</v>
       </c>
       <c r="M31" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="N31" t="n">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="O31" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="32">
@@ -2067,10 +2163,13 @@
         <v>1</v>
       </c>
       <c r="M32" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="N32" t="n">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="O32" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="33">
@@ -2117,10 +2216,13 @@
         <v>1</v>
       </c>
       <c r="M33" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="N33" t="n">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="O33" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="34">
@@ -2167,11 +2269,14 @@
         <v>1</v>
       </c>
       <c r="M34" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="N34" t="n">
         <v>6</v>
       </c>
+      <c r="O34" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -2217,11 +2322,14 @@
         <v>1</v>
       </c>
       <c r="M35" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N35" t="n">
         <v>5</v>
       </c>
+      <c r="O35" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -2267,10 +2375,13 @@
         <v>1</v>
       </c>
       <c r="M36" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="N36" t="n">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="O36" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="37">
@@ -2317,11 +2428,14 @@
         <v>1</v>
       </c>
       <c r="M37" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N37" t="n">
         <v>3</v>
       </c>
+      <c r="O37" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -2372,6 +2486,9 @@
       <c r="N38" t="n">
         <v>0</v>
       </c>
+      <c r="O38" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -2422,6 +2539,9 @@
       <c r="N39" t="n">
         <v>0</v>
       </c>
+      <c r="O39" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -2467,10 +2587,13 @@
         <v>1</v>
       </c>
       <c r="M40" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="N40" t="n">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="O40" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="41">
@@ -2517,10 +2640,13 @@
         <v>1</v>
       </c>
       <c r="M41" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="N41" t="n">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="O41" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="42">
@@ -2567,10 +2693,13 @@
         <v>1</v>
       </c>
       <c r="M42" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="N42" t="n">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="O42" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="43">
@@ -2617,9 +2746,12 @@
         <v>0</v>
       </c>
       <c r="M43" t="n">
+        <v>0</v>
+      </c>
+      <c r="N43" t="n">
         <v>21</v>
       </c>
-      <c r="N43" t="n">
+      <c r="O43" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2667,10 +2799,13 @@
         <v>1</v>
       </c>
       <c r="M44" t="n">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="N44" t="n">
-        <v>3</v>
+        <v>45</v>
+      </c>
+      <c r="O44" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="45">
@@ -2717,10 +2852,13 @@
         <v>1</v>
       </c>
       <c r="M45" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N45" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="O45" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="46">
@@ -2767,10 +2905,13 @@
         <v>1</v>
       </c>
       <c r="M46" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="N46" t="n">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="O46" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="47">
@@ -2817,11 +2958,14 @@
         <v>1</v>
       </c>
       <c r="M47" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="N47" t="n">
         <v>6</v>
       </c>
+      <c r="O47" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -2872,6 +3016,9 @@
       <c r="N48" t="n">
         <v>0</v>
       </c>
+      <c r="O48" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2917,11 +3064,14 @@
         <v>1</v>
       </c>
       <c r="M49" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="N49" t="n">
         <v>6</v>
       </c>
+      <c r="O49" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -2967,10 +3117,13 @@
         <v>1</v>
       </c>
       <c r="M50" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="N50" t="n">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="O50" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="51">
@@ -3020,7 +3173,10 @@
         <v>1</v>
       </c>
       <c r="N51" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="O51" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="52">
@@ -3067,10 +3223,13 @@
         <v>0</v>
       </c>
       <c r="M52" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N52" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="O52" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="53">
@@ -3117,10 +3276,13 @@
         <v>1</v>
       </c>
       <c r="M53" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="N53" t="n">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="O53" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="54">
@@ -3172,6 +3334,9 @@
       <c r="N54" t="n">
         <v>0</v>
       </c>
+      <c r="O54" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -3217,11 +3382,14 @@
         <v>1</v>
       </c>
       <c r="M55" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="N55" t="n">
         <v>6</v>
       </c>
+      <c r="O55" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -3272,6 +3440,9 @@
       <c r="N56" t="n">
         <v>0</v>
       </c>
+      <c r="O56" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -3317,10 +3488,13 @@
         <v>1</v>
       </c>
       <c r="M57" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="N57" t="n">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="O57" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="58">
@@ -3367,10 +3541,13 @@
         <v>1</v>
       </c>
       <c r="M58" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="N58" t="n">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="O58" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="59">
@@ -3417,11 +3594,14 @@
         <v>0</v>
       </c>
       <c r="M59" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N59" t="n">
         <v>3</v>
       </c>
+      <c r="O59" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -3467,10 +3647,13 @@
         <v>1</v>
       </c>
       <c r="M60" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="N60" t="n">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="O60" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="61">
@@ -3517,9 +3700,12 @@
         <v>0</v>
       </c>
       <c r="M61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N61" t="n">
+        <v>1</v>
+      </c>
+      <c r="O61" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3572,6 +3758,9 @@
       <c r="N62" t="n">
         <v>0</v>
       </c>
+      <c r="O62" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -3617,10 +3806,13 @@
         <v>1</v>
       </c>
       <c r="M63" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N63" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="O63" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="64">
@@ -3667,10 +3859,13 @@
         <v>1</v>
       </c>
       <c r="M64" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="N64" t="n">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="O64" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="65">
@@ -3722,6 +3917,9 @@
       <c r="N65" t="n">
         <v>0</v>
       </c>
+      <c r="O65" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -3772,6 +3970,9 @@
       <c r="N66" t="n">
         <v>0</v>
       </c>
+      <c r="O66" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -3817,10 +4018,13 @@
         <v>0</v>
       </c>
       <c r="M67" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N67" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="O67" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="68">
@@ -3872,6 +4076,9 @@
       <c r="N68" t="n">
         <v>0</v>
       </c>
+      <c r="O68" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -3922,6 +4129,9 @@
       <c r="N69" t="n">
         <v>0</v>
       </c>
+      <c r="O69" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -3967,10 +4177,13 @@
         <v>1</v>
       </c>
       <c r="M70" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="N70" t="n">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="O70" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="71">
@@ -4017,9 +4230,12 @@
         <v>0</v>
       </c>
       <c r="M71" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N71" t="n">
+        <v>1</v>
+      </c>
+      <c r="O71" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4072,6 +4288,9 @@
       <c r="N72" t="n">
         <v>0</v>
       </c>
+      <c r="O72" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -4117,11 +4336,14 @@
         <v>1</v>
       </c>
       <c r="M73" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N73" t="n">
         <v>3</v>
       </c>
+      <c r="O73" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -4167,10 +4389,13 @@
         <v>1</v>
       </c>
       <c r="M74" t="n">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="N74" t="n">
-        <v>5</v>
+        <v>18</v>
+      </c>
+      <c r="O74" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="75">
@@ -4220,7 +4445,10 @@
         <v>1</v>
       </c>
       <c r="N75" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="O75" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="76">
@@ -4267,10 +4495,13 @@
         <v>1</v>
       </c>
       <c r="M76" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="N76" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="O76" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="77">
@@ -4322,6 +4553,9 @@
       <c r="N77" t="n">
         <v>0</v>
       </c>
+      <c r="O77" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -4372,6 +4606,9 @@
       <c r="N78" t="n">
         <v>0</v>
       </c>
+      <c r="O78" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -4417,11 +4654,14 @@
         <v>1</v>
       </c>
       <c r="M79" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N79" t="n">
         <v>3</v>
       </c>
+      <c r="O79" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -4467,10 +4707,13 @@
         <v>1</v>
       </c>
       <c r="M80" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="N80" t="n">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="O80" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="81">
@@ -4517,10 +4760,13 @@
         <v>0</v>
       </c>
       <c r="M81" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="N81" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="O81" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="82">
@@ -4567,10 +4813,13 @@
         <v>1</v>
       </c>
       <c r="M82" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="N82" t="n">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="O82" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="83">
@@ -4617,10 +4866,13 @@
         <v>1</v>
       </c>
       <c r="M83" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N83" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="O83" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="84">
@@ -4667,9 +4919,12 @@
         <v>0</v>
       </c>
       <c r="M84" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N84" t="n">
+        <v>1</v>
+      </c>
+      <c r="O84" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4722,6 +4977,9 @@
       <c r="N85" t="n">
         <v>0</v>
       </c>
+      <c r="O85" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -4767,10 +5025,13 @@
         <v>1</v>
       </c>
       <c r="M86" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N86" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="O86" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="87">
@@ -4822,6 +5083,9 @@
       <c r="N87" t="n">
         <v>0</v>
       </c>
+      <c r="O87" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -4867,10 +5131,13 @@
         <v>0</v>
       </c>
       <c r="M88" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N88" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="O88" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="89">
@@ -4922,6 +5189,9 @@
       <c r="N89" t="n">
         <v>0</v>
       </c>
+      <c r="O89" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -4967,11 +5237,14 @@
         <v>1</v>
       </c>
       <c r="M90" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N90" t="n">
         <v>2</v>
       </c>
+      <c r="O90" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -5022,6 +5295,9 @@
       <c r="N91" t="n">
         <v>0</v>
       </c>
+      <c r="O91" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -5072,6 +5348,9 @@
       <c r="N92" t="n">
         <v>0</v>
       </c>
+      <c r="O92" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -5117,10 +5396,13 @@
         <v>1</v>
       </c>
       <c r="M93" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N93" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="O93" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="94">
@@ -5167,10 +5449,13 @@
         <v>1</v>
       </c>
       <c r="M94" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="N94" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="O94" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="95">
@@ -5217,10 +5502,13 @@
         <v>1</v>
       </c>
       <c r="M95" t="n">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="N95" t="n">
-        <v>4</v>
+        <v>34</v>
+      </c>
+      <c r="O95" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="96">
@@ -5270,7 +5558,10 @@
         <v>1</v>
       </c>
       <c r="N96" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="O96" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="97">
@@ -5322,6 +5613,9 @@
       <c r="N97" t="n">
         <v>0</v>
       </c>
+      <c r="O97" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -5367,10 +5661,13 @@
         <v>1</v>
       </c>
       <c r="M98" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N98" t="n">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="O98" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="99">
@@ -5422,6 +5719,9 @@
       <c r="N99" t="n">
         <v>0</v>
       </c>
+      <c r="O99" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -5467,11 +5767,14 @@
         <v>0</v>
       </c>
       <c r="M100" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N100" t="n">
         <v>2</v>
       </c>
+      <c r="O100" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -5517,10 +5820,13 @@
         <v>1</v>
       </c>
       <c r="M101" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="N101" t="n">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="O101" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="102">
@@ -5572,6 +5878,9 @@
       <c r="N102" t="n">
         <v>0</v>
       </c>
+      <c r="O102" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -5617,10 +5926,13 @@
         <v>1</v>
       </c>
       <c r="M103" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="N103" t="n">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="O103" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="104">
@@ -5667,9 +5979,12 @@
         <v>0</v>
       </c>
       <c r="M104" t="n">
+        <v>0</v>
+      </c>
+      <c r="N104" t="n">
         <v>12</v>
       </c>
-      <c r="N104" t="n">
+      <c r="O104" t="n">
         <v>1</v>
       </c>
     </row>
@@ -5717,10 +6032,13 @@
         <v>1</v>
       </c>
       <c r="M105" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="N105" t="n">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="O105" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="106">
@@ -5767,11 +6085,14 @@
         <v>1</v>
       </c>
       <c r="M106" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="N106" t="n">
         <v>6</v>
       </c>
+      <c r="O106" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -5822,6 +6143,9 @@
       <c r="N107" t="n">
         <v>0</v>
       </c>
+      <c r="O107" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -5867,10 +6191,13 @@
         <v>1</v>
       </c>
       <c r="M108" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="N108" t="n">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="O108" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="109">
@@ -5920,6 +6247,9 @@
         <v>0</v>
       </c>
       <c r="N109" t="n">
+        <v>0</v>
+      </c>
+      <c r="O109" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>